<commit_message>
Updated with latest figures
</commit_message>
<xml_diff>
--- a/Indian COVID-19 Infection Projections.xlsx
+++ b/Indian COVID-19 Infection Projections.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python\Aus COVID-19 Projections\Aus-COVID-19-Projections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B316C82-D52A-46E7-B4C9-5D70FEE389A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A805BCCE-9681-4809-AA2C-7B77B38E376B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{744C986A-0D24-487A-A5C2-8E2494A78887}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{744C986A-0D24-487A-A5C2-8E2494A78887}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="4" r:id="rId1"/>
@@ -1397,6 +1397,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="15" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="16" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="6" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="15" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="6" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="6" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1421,22 +1437,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="15" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="16" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="6" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="15" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="6" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="6" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Heading" xfId="3" xr:uid="{DB9EF5E1-A693-41C3-82C7-CA90563DBB00}"/>
@@ -1759,46 +1759,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43894.680232754632</c:v>
+                  <c:v>43895.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43897.680232754632</c:v>
+                  <c:v>43898.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43900.680232754632</c:v>
+                  <c:v>43901.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43903.680232754632</c:v>
+                  <c:v>43904.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43906.680232754632</c:v>
+                  <c:v>43907.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43909.680232754632</c:v>
+                  <c:v>43910.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43912.680232754632</c:v>
+                  <c:v>43913.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43915.680232754632</c:v>
+                  <c:v>43916.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43918.680232754632</c:v>
+                  <c:v>43919.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43921.680232754632</c:v>
+                  <c:v>43922.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43924.680232754632</c:v>
+                  <c:v>43925.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43927.680232754632</c:v>
+                  <c:v>43928.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43930.680232754632</c:v>
+                  <c:v>43931.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43933.680232754632</c:v>
+                  <c:v>43934.47386273148</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1908,46 +1908,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43894.680232754632</c:v>
+                  <c:v>43895.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43897.680232754632</c:v>
+                  <c:v>43898.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43900.680232754632</c:v>
+                  <c:v>43901.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43903.680232754632</c:v>
+                  <c:v>43904.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43906.680232754632</c:v>
+                  <c:v>43907.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43909.680232754632</c:v>
+                  <c:v>43910.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43912.680232754632</c:v>
+                  <c:v>43913.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43915.680232754632</c:v>
+                  <c:v>43916.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43918.680232754632</c:v>
+                  <c:v>43919.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43921.680232754632</c:v>
+                  <c:v>43922.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43924.680232754632</c:v>
+                  <c:v>43925.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43927.680232754632</c:v>
+                  <c:v>43928.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43930.680232754632</c:v>
+                  <c:v>43931.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43933.680232754632</c:v>
+                  <c:v>43934.47386273148</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2057,46 +2057,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43894.680232754632</c:v>
+                  <c:v>43895.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43897.680232754632</c:v>
+                  <c:v>43898.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43900.680232754632</c:v>
+                  <c:v>43901.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43903.680232754632</c:v>
+                  <c:v>43904.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43906.680232754632</c:v>
+                  <c:v>43907.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43909.680232754632</c:v>
+                  <c:v>43910.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43912.680232754632</c:v>
+                  <c:v>43913.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43915.680232754632</c:v>
+                  <c:v>43916.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43918.680232754632</c:v>
+                  <c:v>43919.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43921.680232754632</c:v>
+                  <c:v>43922.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43924.680232754632</c:v>
+                  <c:v>43925.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43927.680232754632</c:v>
+                  <c:v>43928.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43930.680232754632</c:v>
+                  <c:v>43931.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43933.680232754632</c:v>
+                  <c:v>43934.47386273148</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3202,7 +3202,7 @@
                   <c:v>249</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="#,##0">
-                  <c:v>331</c:v>
+                  <c:v>358</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12411,7 +12411,7 @@
                   <c:v>249</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="#,##0">
-                  <c:v>331</c:v>
+                  <c:v>358</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12740,46 +12740,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43894.680232754632</c:v>
+                  <c:v>43895.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43897.680232754632</c:v>
+                  <c:v>43898.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43900.680232754632</c:v>
+                  <c:v>43901.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43903.680232754632</c:v>
+                  <c:v>43904.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43906.680232754632</c:v>
+                  <c:v>43907.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43909.680232754632</c:v>
+                  <c:v>43910.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43912.680232754632</c:v>
+                  <c:v>43913.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43915.680232754632</c:v>
+                  <c:v>43916.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43918.680232754632</c:v>
+                  <c:v>43919.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43921.680232754632</c:v>
+                  <c:v>43922.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43924.680232754632</c:v>
+                  <c:v>43925.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43927.680232754632</c:v>
+                  <c:v>43928.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43930.680232754632</c:v>
+                  <c:v>43931.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43933.680232754632</c:v>
+                  <c:v>43934.47386273148</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12880,46 +12880,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43894.680232754632</c:v>
+                  <c:v>43895.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43897.680232754632</c:v>
+                  <c:v>43898.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43900.680232754632</c:v>
+                  <c:v>43901.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43903.680232754632</c:v>
+                  <c:v>43904.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43906.680232754632</c:v>
+                  <c:v>43907.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43909.680232754632</c:v>
+                  <c:v>43910.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43912.680232754632</c:v>
+                  <c:v>43913.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43915.680232754632</c:v>
+                  <c:v>43916.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43918.680232754632</c:v>
+                  <c:v>43919.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43921.680232754632</c:v>
+                  <c:v>43922.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43924.680232754632</c:v>
+                  <c:v>43925.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43927.680232754632</c:v>
+                  <c:v>43928.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43930.680232754632</c:v>
+                  <c:v>43931.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43933.680232754632</c:v>
+                  <c:v>43934.47386273148</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13023,46 +13023,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43894.680232754632</c:v>
+                  <c:v>43895.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43897.680232754632</c:v>
+                  <c:v>43898.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43900.680232754632</c:v>
+                  <c:v>43901.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43903.680232754632</c:v>
+                  <c:v>43904.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43906.680232754632</c:v>
+                  <c:v>43907.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43909.680232754632</c:v>
+                  <c:v>43910.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43912.680232754632</c:v>
+                  <c:v>43913.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43915.680232754632</c:v>
+                  <c:v>43916.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43918.680232754632</c:v>
+                  <c:v>43919.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43921.680232754632</c:v>
+                  <c:v>43922.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43924.680232754632</c:v>
+                  <c:v>43925.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43927.680232754632</c:v>
+                  <c:v>43928.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43930.680232754632</c:v>
+                  <c:v>43931.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43933.680232754632</c:v>
+                  <c:v>43934.47386273148</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13160,46 +13160,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43894.680232754632</c:v>
+                  <c:v>43895.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43897.680232754632</c:v>
+                  <c:v>43898.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43900.680232754632</c:v>
+                  <c:v>43901.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43903.680232754632</c:v>
+                  <c:v>43904.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43906.680232754632</c:v>
+                  <c:v>43907.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43909.680232754632</c:v>
+                  <c:v>43910.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43912.680232754632</c:v>
+                  <c:v>43913.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43915.680232754632</c:v>
+                  <c:v>43916.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43918.680232754632</c:v>
+                  <c:v>43919.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43921.680232754632</c:v>
+                  <c:v>43922.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43924.680232754632</c:v>
+                  <c:v>43925.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43927.680232754632</c:v>
+                  <c:v>43928.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43930.680232754632</c:v>
+                  <c:v>43931.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43933.680232754632</c:v>
+                  <c:v>43934.47386273148</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13567,46 +13567,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43894.680232754632</c:v>
+                  <c:v>43895.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43897.680232754632</c:v>
+                  <c:v>43898.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43900.680232754632</c:v>
+                  <c:v>43901.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43903.680232754632</c:v>
+                  <c:v>43904.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43906.680232754632</c:v>
+                  <c:v>43907.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43909.680232754632</c:v>
+                  <c:v>43910.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43912.680232754632</c:v>
+                  <c:v>43913.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43915.680232754632</c:v>
+                  <c:v>43916.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43918.680232754632</c:v>
+                  <c:v>43919.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43921.680232754632</c:v>
+                  <c:v>43922.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43924.680232754632</c:v>
+                  <c:v>43925.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43927.680232754632</c:v>
+                  <c:v>43928.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43930.680232754632</c:v>
+                  <c:v>43931.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43933.680232754632</c:v>
+                  <c:v>43934.47386273148</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13716,46 +13716,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43894.680232754632</c:v>
+                  <c:v>43895.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43897.680232754632</c:v>
+                  <c:v>43898.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43900.680232754632</c:v>
+                  <c:v>43901.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43903.680232754632</c:v>
+                  <c:v>43904.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43906.680232754632</c:v>
+                  <c:v>43907.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43909.680232754632</c:v>
+                  <c:v>43910.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43912.680232754632</c:v>
+                  <c:v>43913.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43915.680232754632</c:v>
+                  <c:v>43916.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43918.680232754632</c:v>
+                  <c:v>43919.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43921.680232754632</c:v>
+                  <c:v>43922.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43924.680232754632</c:v>
+                  <c:v>43925.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43927.680232754632</c:v>
+                  <c:v>43928.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43930.680232754632</c:v>
+                  <c:v>43931.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43933.680232754632</c:v>
+                  <c:v>43934.47386273148</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13865,46 +13865,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43894.680232754632</c:v>
+                  <c:v>43895.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43897.680232754632</c:v>
+                  <c:v>43898.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43900.680232754632</c:v>
+                  <c:v>43901.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43903.680232754632</c:v>
+                  <c:v>43904.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43906.680232754632</c:v>
+                  <c:v>43907.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43909.680232754632</c:v>
+                  <c:v>43910.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43912.680232754632</c:v>
+                  <c:v>43913.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43915.680232754632</c:v>
+                  <c:v>43916.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43918.680232754632</c:v>
+                  <c:v>43919.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43921.680232754632</c:v>
+                  <c:v>43922.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43924.680232754632</c:v>
+                  <c:v>43925.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43927.680232754632</c:v>
+                  <c:v>43928.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43930.680232754632</c:v>
+                  <c:v>43931.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43933.680232754632</c:v>
+                  <c:v>43934.47386273148</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14282,46 +14282,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43894.680232754632</c:v>
+                  <c:v>43895.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43897.680232754632</c:v>
+                  <c:v>43898.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43900.680232754632</c:v>
+                  <c:v>43901.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43903.680232754632</c:v>
+                  <c:v>43904.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43906.680232754632</c:v>
+                  <c:v>43907.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43909.680232754632</c:v>
+                  <c:v>43910.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43912.680232754632</c:v>
+                  <c:v>43913.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43915.680232754632</c:v>
+                  <c:v>43916.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43918.680232754632</c:v>
+                  <c:v>43919.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43921.680232754632</c:v>
+                  <c:v>43922.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43924.680232754632</c:v>
+                  <c:v>43925.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43927.680232754632</c:v>
+                  <c:v>43928.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43930.680232754632</c:v>
+                  <c:v>43931.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43933.680232754632</c:v>
+                  <c:v>43934.47386273148</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14422,46 +14422,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43894.680232754632</c:v>
+                  <c:v>43895.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43897.680232754632</c:v>
+                  <c:v>43898.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43900.680232754632</c:v>
+                  <c:v>43901.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43903.680232754632</c:v>
+                  <c:v>43904.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43906.680232754632</c:v>
+                  <c:v>43907.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43909.680232754632</c:v>
+                  <c:v>43910.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43912.680232754632</c:v>
+                  <c:v>43913.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43915.680232754632</c:v>
+                  <c:v>43916.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43918.680232754632</c:v>
+                  <c:v>43919.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43921.680232754632</c:v>
+                  <c:v>43922.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43924.680232754632</c:v>
+                  <c:v>43925.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43927.680232754632</c:v>
+                  <c:v>43928.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43930.680232754632</c:v>
+                  <c:v>43931.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43933.680232754632</c:v>
+                  <c:v>43934.47386273148</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14565,46 +14565,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43894.680232754632</c:v>
+                  <c:v>43895.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43897.680232754632</c:v>
+                  <c:v>43898.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43900.680232754632</c:v>
+                  <c:v>43901.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43903.680232754632</c:v>
+                  <c:v>43904.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43906.680232754632</c:v>
+                  <c:v>43907.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43909.680232754632</c:v>
+                  <c:v>43910.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43912.680232754632</c:v>
+                  <c:v>43913.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43915.680232754632</c:v>
+                  <c:v>43916.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43918.680232754632</c:v>
+                  <c:v>43919.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43921.680232754632</c:v>
+                  <c:v>43922.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43924.680232754632</c:v>
+                  <c:v>43925.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43927.680232754632</c:v>
+                  <c:v>43928.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43930.680232754632</c:v>
+                  <c:v>43931.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43933.680232754632</c:v>
+                  <c:v>43934.47386273148</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14702,46 +14702,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43894.680232754632</c:v>
+                  <c:v>43895.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43897.680232754632</c:v>
+                  <c:v>43898.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43900.680232754632</c:v>
+                  <c:v>43901.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43903.680232754632</c:v>
+                  <c:v>43904.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43906.680232754632</c:v>
+                  <c:v>43907.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43909.680232754632</c:v>
+                  <c:v>43910.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43912.680232754632</c:v>
+                  <c:v>43913.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43915.680232754632</c:v>
+                  <c:v>43916.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43918.680232754632</c:v>
+                  <c:v>43919.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43921.680232754632</c:v>
+                  <c:v>43922.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43924.680232754632</c:v>
+                  <c:v>43925.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43927.680232754632</c:v>
+                  <c:v>43928.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43930.680232754632</c:v>
+                  <c:v>43931.47386273148</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43933.680232754632</c:v>
+                  <c:v>43934.47386273148</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -34893,167 +34893,167 @@
       </c>
       <c r="B26" s="83">
         <f t="shared" ref="B26:G26" ca="1" si="0">C26-1</f>
-        <v>43894.680232754632</v>
+        <v>43895.47386273148</v>
       </c>
       <c r="C26" s="84">
         <f t="shared" ca="1" si="0"/>
-        <v>43895.680232754632</v>
+        <v>43896.47386273148</v>
       </c>
       <c r="D26" s="84">
         <f t="shared" ca="1" si="0"/>
-        <v>43896.680232754632</v>
+        <v>43897.47386273148</v>
       </c>
       <c r="E26" s="84">
         <f t="shared" ca="1" si="0"/>
-        <v>43897.680232754632</v>
+        <v>43898.47386273148</v>
       </c>
       <c r="F26" s="84">
         <f t="shared" ca="1" si="0"/>
-        <v>43898.680232754632</v>
+        <v>43899.47386273148</v>
       </c>
       <c r="G26" s="85">
         <f t="shared" ca="1" si="0"/>
-        <v>43899.680232754632</v>
+        <v>43900.47386273148</v>
       </c>
       <c r="H26" s="84">
         <f t="shared" ref="H26:U26" ca="1" si="1">I26-1</f>
-        <v>43900.680232754632</v>
+        <v>43901.47386273148</v>
       </c>
       <c r="I26" s="84">
         <f t="shared" ca="1" si="1"/>
-        <v>43901.680232754632</v>
+        <v>43902.47386273148</v>
       </c>
       <c r="J26" s="84">
         <f t="shared" ca="1" si="1"/>
-        <v>43902.680232754632</v>
+        <v>43903.47386273148</v>
       </c>
       <c r="K26" s="84">
         <f t="shared" ca="1" si="1"/>
-        <v>43903.680232754632</v>
+        <v>43904.47386273148</v>
       </c>
       <c r="L26" s="84">
         <f t="shared" ca="1" si="1"/>
-        <v>43904.680232754632</v>
+        <v>43905.47386273148</v>
       </c>
       <c r="M26" s="84">
         <f t="shared" ca="1" si="1"/>
-        <v>43905.680232754632</v>
+        <v>43906.47386273148</v>
       </c>
       <c r="N26" s="85">
         <f t="shared" ca="1" si="1"/>
-        <v>43906.680232754632</v>
+        <v>43907.47386273148</v>
       </c>
       <c r="O26" s="83">
         <f t="shared" ca="1" si="1"/>
-        <v>43907.680232754632</v>
+        <v>43908.47386273148</v>
       </c>
       <c r="P26" s="84">
         <f t="shared" ca="1" si="1"/>
-        <v>43908.680232754632</v>
+        <v>43909.47386273148</v>
       </c>
       <c r="Q26" s="84">
         <f t="shared" ca="1" si="1"/>
-        <v>43909.680232754632</v>
+        <v>43910.47386273148</v>
       </c>
       <c r="R26" s="84">
         <f t="shared" ca="1" si="1"/>
-        <v>43910.680232754632</v>
+        <v>43911.47386273148</v>
       </c>
       <c r="S26" s="84">
         <f t="shared" ca="1" si="1"/>
-        <v>43911.680232754632</v>
+        <v>43912.47386273148</v>
       </c>
       <c r="T26" s="84">
         <f t="shared" ca="1" si="1"/>
-        <v>43912.680232754632</v>
+        <v>43913.47386273148</v>
       </c>
       <c r="U26" s="85">
         <f t="shared" ca="1" si="1"/>
-        <v>43913.680232754632</v>
+        <v>43914.47386273148</v>
       </c>
       <c r="V26" s="83">
         <f t="shared" ref="V26:AN26" ca="1" si="2">W26-1</f>
-        <v>43914.680232754632</v>
+        <v>43915.47386273148</v>
       </c>
       <c r="W26" s="84">
         <f t="shared" ca="1" si="2"/>
-        <v>43915.680232754632</v>
+        <v>43916.47386273148</v>
       </c>
       <c r="X26" s="84">
         <f t="shared" ca="1" si="2"/>
-        <v>43916.680232754632</v>
+        <v>43917.47386273148</v>
       </c>
       <c r="Y26" s="84">
         <f t="shared" ca="1" si="2"/>
-        <v>43917.680232754632</v>
+        <v>43918.47386273148</v>
       </c>
       <c r="Z26" s="84">
         <f t="shared" ca="1" si="2"/>
-        <v>43918.680232754632</v>
+        <v>43919.47386273148</v>
       </c>
       <c r="AA26" s="84">
         <f t="shared" ca="1" si="2"/>
-        <v>43919.680232754632</v>
+        <v>43920.47386273148</v>
       </c>
       <c r="AB26" s="85">
         <f t="shared" ca="1" si="2"/>
-        <v>43920.680232754632</v>
+        <v>43921.47386273148</v>
       </c>
       <c r="AC26" s="83">
         <f t="shared" ca="1" si="2"/>
-        <v>43921.680232754632</v>
+        <v>43922.47386273148</v>
       </c>
       <c r="AD26" s="84">
         <f t="shared" ca="1" si="2"/>
-        <v>43922.680232754632</v>
+        <v>43923.47386273148</v>
       </c>
       <c r="AE26" s="84">
         <f t="shared" ca="1" si="2"/>
-        <v>43923.680232754632</v>
+        <v>43924.47386273148</v>
       </c>
       <c r="AF26" s="84">
         <f t="shared" ca="1" si="2"/>
-        <v>43924.680232754632</v>
+        <v>43925.47386273148</v>
       </c>
       <c r="AG26" s="84">
         <f t="shared" ca="1" si="2"/>
-        <v>43925.680232754632</v>
+        <v>43926.47386273148</v>
       </c>
       <c r="AH26" s="84">
         <f t="shared" ca="1" si="2"/>
-        <v>43926.680232754632</v>
+        <v>43927.47386273148</v>
       </c>
       <c r="AI26" s="85">
         <f t="shared" ca="1" si="2"/>
-        <v>43927.680232754632</v>
+        <v>43928.47386273148</v>
       </c>
       <c r="AJ26" s="83">
         <f t="shared" ca="1" si="2"/>
-        <v>43928.680232754632</v>
+        <v>43929.47386273148</v>
       </c>
       <c r="AK26" s="84">
         <f t="shared" ca="1" si="2"/>
-        <v>43929.680232754632</v>
+        <v>43930.47386273148</v>
       </c>
       <c r="AL26" s="84">
         <f t="shared" ca="1" si="2"/>
-        <v>43930.680232754632</v>
+        <v>43931.47386273148</v>
       </c>
       <c r="AM26" s="84">
         <f t="shared" ca="1" si="2"/>
-        <v>43931.680232754632</v>
+        <v>43932.47386273148</v>
       </c>
       <c r="AN26" s="84">
         <f t="shared" ca="1" si="2"/>
-        <v>43932.680232754632</v>
+        <v>43933.47386273148</v>
       </c>
       <c r="AO26" s="84">
         <f ca="1">AP26-1</f>
-        <v>43933.680232754632</v>
+        <v>43934.47386273148</v>
       </c>
       <c r="AP26" s="105">
         <f ca="1">NOW()</f>
-        <v>43934.680232754632</v>
+        <v>43935.47386273148</v>
       </c>
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.25">
@@ -35188,59 +35188,59 @@
       <c r="A28" s="129" t="s">
         <v>98</v>
       </c>
-      <c r="B28" s="275" t="s">
+      <c r="B28" s="289" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="276"/>
-      <c r="D28" s="276"/>
-      <c r="E28" s="276"/>
-      <c r="F28" s="276"/>
-      <c r="G28" s="277"/>
-      <c r="H28" s="281" t="s">
+      <c r="C28" s="290"/>
+      <c r="D28" s="290"/>
+      <c r="E28" s="290"/>
+      <c r="F28" s="290"/>
+      <c r="G28" s="291"/>
+      <c r="H28" s="295" t="s">
         <v>56</v>
       </c>
-      <c r="I28" s="281"/>
-      <c r="J28" s="281"/>
-      <c r="K28" s="281"/>
-      <c r="L28" s="281"/>
-      <c r="M28" s="281"/>
-      <c r="N28" s="282"/>
-      <c r="O28" s="280" t="s">
+      <c r="I28" s="295"/>
+      <c r="J28" s="295"/>
+      <c r="K28" s="295"/>
+      <c r="L28" s="295"/>
+      <c r="M28" s="295"/>
+      <c r="N28" s="296"/>
+      <c r="O28" s="294" t="s">
         <v>57</v>
       </c>
-      <c r="P28" s="281"/>
-      <c r="Q28" s="281"/>
-      <c r="R28" s="281"/>
-      <c r="S28" s="281"/>
-      <c r="T28" s="281"/>
-      <c r="U28" s="282"/>
-      <c r="V28" s="280" t="s">
+      <c r="P28" s="295"/>
+      <c r="Q28" s="295"/>
+      <c r="R28" s="295"/>
+      <c r="S28" s="295"/>
+      <c r="T28" s="295"/>
+      <c r="U28" s="296"/>
+      <c r="V28" s="294" t="s">
         <v>58</v>
       </c>
-      <c r="W28" s="281"/>
-      <c r="X28" s="281"/>
-      <c r="Y28" s="281"/>
-      <c r="Z28" s="281"/>
-      <c r="AA28" s="281"/>
-      <c r="AB28" s="282"/>
-      <c r="AC28" s="280" t="s">
+      <c r="W28" s="295"/>
+      <c r="X28" s="295"/>
+      <c r="Y28" s="295"/>
+      <c r="Z28" s="295"/>
+      <c r="AA28" s="295"/>
+      <c r="AB28" s="296"/>
+      <c r="AC28" s="294" t="s">
         <v>59</v>
       </c>
-      <c r="AD28" s="281"/>
-      <c r="AE28" s="281"/>
-      <c r="AF28" s="281"/>
-      <c r="AG28" s="281"/>
-      <c r="AH28" s="281"/>
-      <c r="AI28" s="282"/>
-      <c r="AJ28" s="280" t="s">
+      <c r="AD28" s="295"/>
+      <c r="AE28" s="295"/>
+      <c r="AF28" s="295"/>
+      <c r="AG28" s="295"/>
+      <c r="AH28" s="295"/>
+      <c r="AI28" s="296"/>
+      <c r="AJ28" s="294" t="s">
         <v>60</v>
       </c>
-      <c r="AK28" s="281"/>
-      <c r="AL28" s="281"/>
-      <c r="AM28" s="281"/>
-      <c r="AN28" s="281"/>
-      <c r="AO28" s="281"/>
-      <c r="AP28" s="282"/>
+      <c r="AK28" s="295"/>
+      <c r="AL28" s="295"/>
+      <c r="AM28" s="295"/>
+      <c r="AN28" s="295"/>
+      <c r="AO28" s="295"/>
+      <c r="AP28" s="296"/>
     </row>
     <row r="29" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B29" s="51" t="s">
@@ -35251,43 +35251,43 @@
       <c r="E29" s="90"/>
       <c r="F29" s="90"/>
       <c r="G29" s="91"/>
-      <c r="H29" s="278" t="s">
+      <c r="H29" s="292" t="s">
         <v>66</v>
       </c>
-      <c r="I29" s="278"/>
-      <c r="J29" s="278"/>
-      <c r="K29" s="278"/>
-      <c r="L29" s="278"/>
-      <c r="M29" s="278"/>
-      <c r="N29" s="278"/>
-      <c r="O29" s="278"/>
-      <c r="P29" s="278"/>
-      <c r="Q29" s="278"/>
-      <c r="R29" s="278"/>
-      <c r="S29" s="278"/>
-      <c r="T29" s="278"/>
-      <c r="U29" s="278"/>
-      <c r="V29" s="278"/>
-      <c r="W29" s="278"/>
-      <c r="X29" s="278"/>
-      <c r="Y29" s="278"/>
-      <c r="Z29" s="278"/>
-      <c r="AA29" s="278"/>
-      <c r="AB29" s="278"/>
-      <c r="AC29" s="278"/>
-      <c r="AD29" s="278"/>
-      <c r="AE29" s="278"/>
-      <c r="AF29" s="278"/>
-      <c r="AG29" s="278"/>
-      <c r="AH29" s="278"/>
-      <c r="AI29" s="278"/>
-      <c r="AJ29" s="278"/>
-      <c r="AK29" s="278"/>
-      <c r="AL29" s="278"/>
-      <c r="AM29" s="278"/>
-      <c r="AN29" s="278"/>
-      <c r="AO29" s="278"/>
-      <c r="AP29" s="279"/>
+      <c r="I29" s="292"/>
+      <c r="J29" s="292"/>
+      <c r="K29" s="292"/>
+      <c r="L29" s="292"/>
+      <c r="M29" s="292"/>
+      <c r="N29" s="292"/>
+      <c r="O29" s="292"/>
+      <c r="P29" s="292"/>
+      <c r="Q29" s="292"/>
+      <c r="R29" s="292"/>
+      <c r="S29" s="292"/>
+      <c r="T29" s="292"/>
+      <c r="U29" s="292"/>
+      <c r="V29" s="292"/>
+      <c r="W29" s="292"/>
+      <c r="X29" s="292"/>
+      <c r="Y29" s="292"/>
+      <c r="Z29" s="292"/>
+      <c r="AA29" s="292"/>
+      <c r="AB29" s="292"/>
+      <c r="AC29" s="292"/>
+      <c r="AD29" s="292"/>
+      <c r="AE29" s="292"/>
+      <c r="AF29" s="292"/>
+      <c r="AG29" s="292"/>
+      <c r="AH29" s="292"/>
+      <c r="AI29" s="292"/>
+      <c r="AJ29" s="292"/>
+      <c r="AK29" s="292"/>
+      <c r="AL29" s="292"/>
+      <c r="AM29" s="292"/>
+      <c r="AN29" s="292"/>
+      <c r="AO29" s="292"/>
+      <c r="AP29" s="293"/>
     </row>
     <row r="31" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B31" s="56" t="s">
@@ -35571,8 +35571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9BB0FAD-39ED-4D53-8BC6-75164ED434B0}">
   <dimension ref="A1:AN93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V46" sqref="V46"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36018,9 +36018,9 @@
         <v>43860</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="283">
-        <f>(AD17-J17)/(LOG(AD18/J18)/LOG(2))</f>
-        <v>7.8</v>
+      <c r="D14" s="275">
+        <f>(AE17-J17)/(LOG(AE18/J18)/LOG(2))</f>
+        <v>7.9047619047619051</v>
       </c>
       <c r="E14" s="164"/>
       <c r="M14" s="16"/>
@@ -36511,91 +36511,91 @@
       <c r="G20" s="16"/>
       <c r="H20" s="16"/>
       <c r="I20" s="16"/>
-      <c r="J20" s="284">
+      <c r="J20" s="276">
         <f t="shared" ref="J20:S20" si="8">MAX(J18-(J26-J27)-(J28-J29)-(J30-J31),0)</f>
         <v>25.016129564011877</v>
       </c>
-      <c r="K20" s="285">
+      <c r="K20" s="277">
         <f t="shared" si="8"/>
         <v>52.366135481904664</v>
       </c>
-      <c r="L20" s="285">
+      <c r="L20" s="277">
         <f t="shared" si="8"/>
         <v>108.52625208919129</v>
       </c>
-      <c r="M20" s="285">
+      <c r="M20" s="277">
         <f t="shared" si="8"/>
         <v>222.10422027875339</v>
       </c>
-      <c r="N20" s="285">
+      <c r="N20" s="277">
         <f>MAX(N18-(N26-N27)-(N28-N29)-(N30-N31),0)</f>
         <v>447.6875</v>
       </c>
-      <c r="O20" s="285">
+      <c r="O20" s="277">
         <f t="shared" si="8"/>
         <v>906.49780135330877</v>
       </c>
-      <c r="P20" s="285">
+      <c r="P20" s="277">
         <f t="shared" si="8"/>
         <v>1856.4333005675624</v>
       </c>
-      <c r="Q20" s="285">
+      <c r="Q20" s="277">
         <f t="shared" si="8"/>
         <v>3721.4155453634608</v>
       </c>
-      <c r="R20" s="285">
+      <c r="R20" s="277">
         <f t="shared" si="8"/>
         <v>7285.310658734079</v>
       </c>
-      <c r="S20" s="285">
+      <c r="S20" s="277">
         <f t="shared" si="8"/>
         <v>11484.268999904449</v>
       </c>
-      <c r="T20" s="285">
+      <c r="T20" s="277">
         <f>MAX(T18-(T26-T27)-(T28-T29)-(T30-T31),0)</f>
         <v>14845.631764669319</v>
       </c>
-      <c r="U20" s="285">
+      <c r="U20" s="277">
         <f t="shared" ref="U20:AJ20" si="9">MAX(U18-(U26-U27)-(U28-U29)-(U30-U31),0)</f>
         <v>33152.076243296273</v>
       </c>
-      <c r="V20" s="285">
+      <c r="V20" s="277">
         <f t="shared" si="9"/>
         <v>69821.885172049617</v>
       </c>
-      <c r="W20" s="285">
+      <c r="W20" s="277">
         <f t="shared" si="9"/>
         <v>143378.69979450261</v>
       </c>
-      <c r="X20" s="285">
+      <c r="X20" s="277">
         <f t="shared" si="9"/>
         <v>295564.10020469577</v>
       </c>
-      <c r="Y20" s="285">
+      <c r="Y20" s="277">
         <f t="shared" si="9"/>
         <v>603858.13694918051</v>
       </c>
-      <c r="Z20" s="285">
+      <c r="Z20" s="277">
         <f t="shared" si="9"/>
         <v>1227070.1135663358</v>
       </c>
-      <c r="AA20" s="285">
+      <c r="AA20" s="277">
         <f t="shared" si="9"/>
         <v>2484620.7802082496</v>
       </c>
-      <c r="AB20" s="285">
+      <c r="AB20" s="277">
         <f t="shared" si="9"/>
         <v>5018539.1947045205</v>
       </c>
-      <c r="AC20" s="285">
+      <c r="AC20" s="277">
         <f t="shared" si="9"/>
         <v>10118500.107672125</v>
       </c>
-      <c r="AD20" s="285">
+      <c r="AD20" s="277">
         <f t="shared" ref="AD20:AI20" si="10">MAX(AD18-(AD26-AD27)-(AD28-AD29)-(AD30-AD31),0)</f>
         <v>20373793.735732064</v>
       </c>
-      <c r="AE20" s="285">
+      <c r="AE20" s="277">
         <f t="shared" si="10"/>
         <v>40980694.441284448</v>
       </c>
@@ -37651,7 +37651,7 @@
       <c r="H29" s="39"/>
       <c r="I29" s="62"/>
       <c r="J29" s="192">
-        <f t="shared" ref="J29:S29" si="32">J28</f>
+        <f t="shared" ref="J29:R29" si="32">J28</f>
         <v>2.8870253994390738</v>
       </c>
       <c r="K29" s="193">
@@ -37687,7 +37687,7 @@
         <v>539.69701610130301</v>
       </c>
       <c r="S29" s="184">
-        <f t="shared" ref="R29:AJ29" si="33">MAX(S28-($J$18*$B$11)*(2^(((S17 - 42) - $J$17)/HLOOKUP((S17-42)-$B$14,$J$41:$AK$43,3,TRUE)))-S31,0)</f>
+        <f t="shared" ref="S29:AJ29" si="33">MAX(S28-($J$18*$B$11)*(2^(((S17 - 42) - $J$17)/HLOOKUP((S17-42)-$B$14,$J$41:$AK$43,3,TRUE)))-S31,0)</f>
         <v>2123.7978702121991</v>
       </c>
       <c r="T29" s="184">
@@ -38737,7 +38737,7 @@
         <f t="shared" si="46"/>
         <v>11.571428571428571</v>
       </c>
-      <c r="T40" s="293">
+      <c r="T40" s="285">
         <f t="shared" si="46"/>
         <v>13</v>
       </c>
@@ -38749,7 +38749,7 @@
         <f t="shared" si="46"/>
         <v>15.857142857142858</v>
       </c>
-      <c r="W40" s="293">
+      <c r="W40" s="285">
         <f t="shared" si="46"/>
         <v>17.285714285714285</v>
       </c>
@@ -38777,7 +38777,7 @@
         <f t="shared" si="46"/>
         <v>25.857142857142858</v>
       </c>
-      <c r="AD40" s="293">
+      <c r="AD40" s="285">
         <f t="shared" ref="AD40:AI40" si="47">(AD17-$B$14)/7</f>
         <v>27.285714285714285</v>
       </c>
@@ -39188,52 +39188,52 @@
       <c r="G44" s="16"/>
       <c r="H44" s="16"/>
       <c r="I44" s="16"/>
-      <c r="J44" s="286">
+      <c r="J44" s="278">
         <v>27</v>
       </c>
-      <c r="K44" s="287">
+      <c r="K44" s="279">
         <v>58</v>
       </c>
-      <c r="L44" s="287">
+      <c r="L44" s="279">
         <v>99</v>
       </c>
-      <c r="M44" s="287">
+      <c r="M44" s="279">
         <v>221</v>
       </c>
-      <c r="N44" s="287">
+      <c r="N44" s="279">
         <v>486</v>
       </c>
-      <c r="O44" s="287">
+      <c r="O44" s="279">
         <v>879</v>
       </c>
-      <c r="P44" s="287">
+      <c r="P44" s="279">
         <v>1792</v>
       </c>
-      <c r="Q44" s="287">
+      <c r="Q44" s="279">
         <v>3843</v>
       </c>
-      <c r="R44" s="287">
+      <c r="R44" s="279">
         <v>6577</v>
       </c>
-      <c r="S44" s="294"/>
-      <c r="T44" s="294"/>
-      <c r="U44" s="294"/>
-      <c r="V44" s="294"/>
-      <c r="W44" s="294"/>
-      <c r="X44" s="294"/>
-      <c r="Y44" s="294"/>
-      <c r="Z44" s="294"/>
-      <c r="AA44" s="294"/>
-      <c r="AB44" s="294"/>
-      <c r="AC44" s="294"/>
-      <c r="AD44" s="294"/>
-      <c r="AE44" s="294"/>
-      <c r="AF44" s="288"/>
-      <c r="AG44" s="288"/>
-      <c r="AH44" s="288"/>
-      <c r="AI44" s="288"/>
-      <c r="AJ44" s="288"/>
-      <c r="AK44" s="289"/>
+      <c r="S44" s="286"/>
+      <c r="T44" s="286"/>
+      <c r="U44" s="286"/>
+      <c r="V44" s="286"/>
+      <c r="W44" s="286"/>
+      <c r="X44" s="286"/>
+      <c r="Y44" s="286"/>
+      <c r="Z44" s="286"/>
+      <c r="AA44" s="286"/>
+      <c r="AB44" s="286"/>
+      <c r="AC44" s="286"/>
+      <c r="AD44" s="286"/>
+      <c r="AE44" s="286"/>
+      <c r="AF44" s="280"/>
+      <c r="AG44" s="280"/>
+      <c r="AH44" s="280"/>
+      <c r="AI44" s="280"/>
+      <c r="AJ44" s="280"/>
+      <c r="AK44" s="281"/>
     </row>
     <row r="45" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A45" s="41" t="s">
@@ -39283,21 +39283,21 @@
         <f t="shared" si="70"/>
         <v>774</v>
       </c>
-      <c r="S45" s="295">
-        <v>1096</v>
-      </c>
-      <c r="T45" s="295"/>
-      <c r="U45" s="295"/>
-      <c r="V45" s="295"/>
-      <c r="W45" s="295"/>
-      <c r="X45" s="295"/>
-      <c r="Y45" s="295"/>
-      <c r="Z45" s="295"/>
-      <c r="AA45" s="295"/>
-      <c r="AB45" s="295"/>
-      <c r="AC45" s="295"/>
-      <c r="AD45" s="295"/>
-      <c r="AE45" s="295"/>
+      <c r="S45" s="287">
+        <v>1181</v>
+      </c>
+      <c r="T45" s="287"/>
+      <c r="U45" s="287"/>
+      <c r="V45" s="287"/>
+      <c r="W45" s="287"/>
+      <c r="X45" s="287"/>
+      <c r="Y45" s="287"/>
+      <c r="Z45" s="287"/>
+      <c r="AA45" s="287"/>
+      <c r="AB45" s="287"/>
+      <c r="AC45" s="287"/>
+      <c r="AD45" s="287"/>
+      <c r="AE45" s="287"/>
       <c r="AF45" s="101"/>
       <c r="AG45" s="101"/>
       <c r="AH45" s="101"/>
@@ -39317,48 +39317,48 @@
       <c r="G46" s="39"/>
       <c r="H46" s="39"/>
       <c r="I46" s="39"/>
-      <c r="J46" s="290">
+      <c r="J46" s="282">
         <v>0</v>
       </c>
-      <c r="K46" s="291">
+      <c r="K46" s="283">
         <v>0</v>
       </c>
-      <c r="L46" s="292">
+      <c r="L46" s="284">
         <v>2</v>
       </c>
-      <c r="M46" s="292">
+      <c r="M46" s="284">
         <v>5</v>
       </c>
-      <c r="N46" s="292">
+      <c r="N46" s="284">
         <v>10</v>
       </c>
-      <c r="O46" s="292">
+      <c r="O46" s="284">
         <v>24</v>
       </c>
-      <c r="P46" s="292">
+      <c r="P46" s="284">
         <v>58</v>
       </c>
-      <c r="Q46" s="292">
+      <c r="Q46" s="284">
         <v>118</v>
       </c>
-      <c r="R46" s="292">
+      <c r="R46" s="284">
         <v>249</v>
       </c>
-      <c r="S46" s="296">
-        <v>331</v>
-      </c>
-      <c r="T46" s="296"/>
-      <c r="U46" s="296"/>
-      <c r="V46" s="296"/>
-      <c r="W46" s="296"/>
-      <c r="X46" s="296"/>
-      <c r="Y46" s="296"/>
-      <c r="Z46" s="296"/>
-      <c r="AA46" s="296"/>
-      <c r="AB46" s="296"/>
-      <c r="AC46" s="296"/>
-      <c r="AD46" s="296"/>
-      <c r="AE46" s="296"/>
+      <c r="S46" s="288">
+        <v>358</v>
+      </c>
+      <c r="T46" s="288"/>
+      <c r="U46" s="288"/>
+      <c r="V46" s="288"/>
+      <c r="W46" s="288"/>
+      <c r="X46" s="288"/>
+      <c r="Y46" s="288"/>
+      <c r="Z46" s="288"/>
+      <c r="AA46" s="288"/>
+      <c r="AB46" s="288"/>
+      <c r="AC46" s="288"/>
+      <c r="AD46" s="288"/>
+      <c r="AE46" s="288"/>
       <c r="AF46" s="81"/>
       <c r="AG46" s="81"/>
       <c r="AH46" s="81"/>
@@ -44004,7 +44004,7 @@
       </c>
       <c r="C7" s="150">
         <f ca="1">NOW()</f>
-        <v>43934.680232754632</v>
+        <v>43935.47386273148</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
@@ -44013,7 +44013,7 @@
       </c>
       <c r="C8" s="151">
         <f ca="1">C7-C5</f>
-        <v>39.680232754632016</v>
+        <v>40.47386273148004</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -44022,7 +44022,7 @@
       </c>
       <c r="C9" s="153">
         <f ca="1">C8/(LOG(C6/C4)/LOG(2))</f>
-        <v>5.0063380854827333</v>
+        <v>5.1064680419636774</v>
       </c>
       <c r="D9" t="s">
         <v>97</v>
@@ -44064,7 +44064,7 @@
       </c>
       <c r="C13" s="159">
         <f ca="1">(C4/Projections!B6)*(2^(((C7-21)-C5)/C9))</f>
-        <v>4235.0855439665293</v>
+        <v>4483.5527295398042</v>
       </c>
     </row>
     <row r="14" spans="2:10" s="66" customFormat="1" x14ac:dyDescent="0.25">
@@ -44073,7 +44073,7 @@
       </c>
       <c r="C14" s="141">
         <f ca="1">C12-C13</f>
-        <v>73315.934864196737</v>
+        <v>73067.467678623463</v>
       </c>
       <c r="E14" s="155"/>
       <c r="F14" s="156" t="s">
@@ -44097,7 +44097,7 @@
       </c>
       <c r="C16" s="77">
         <f ca="1">(C4*Projections!B10)*(2^(((C7-21)-C5)/C9))</f>
-        <v>336.18109048006318</v>
+        <v>355.9044156708697</v>
       </c>
       <c r="I16" s="149"/>
     </row>
@@ -44107,7 +44107,7 @@
       </c>
       <c r="C17" s="77">
         <f ca="1">C15-C16</f>
-        <v>5819.8189095199368</v>
+        <v>5800.0955843291304</v>
       </c>
       <c r="F17" t="s">
         <v>143</v>
@@ -44129,7 +44129,7 @@
       </c>
       <c r="C19" s="77">
         <f ca="1">(C4*Projections!B11)*(2^(((C7-49)-C5)/C9))</f>
-        <v>1.203878131711227</v>
+        <v>1.3751690199318511</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -44138,7 +44138,7 @@
       </c>
       <c r="C20" s="77">
         <f ca="1">C18-C19</f>
-        <v>1062.7961218682888</v>
+        <v>1062.6248309800681</v>
       </c>
       <c r="F20" t="s">
         <v>148</v>
@@ -44160,7 +44160,7 @@
       </c>
       <c r="C22" s="77">
         <f ca="1">(C4*Projections!B12)*(2^(((C7-49)-C5)/C9))</f>
-        <v>0.42995647561115252</v>
+        <v>0.49113179283280395</v>
       </c>
       <c r="I22" s="149"/>
     </row>
@@ -44170,7 +44170,7 @@
       </c>
       <c r="C23" s="77">
         <f ca="1">C21-C22</f>
-        <v>379.57004352438884</v>
+        <v>379.50886820716721</v>
       </c>
       <c r="I23" s="149"/>
     </row>
@@ -44189,7 +44189,7 @@
       </c>
       <c r="C25" s="60">
         <f ca="1">(C4*Projections!B13)*(2^(((C7-42)-C5)/C9))</f>
-        <v>0.7026266642375002</v>
+        <v>0.78748958075925601</v>
       </c>
       <c r="F25" t="s">
         <v>154</v>
@@ -44201,7 +44201,7 @@
       </c>
       <c r="C26" s="162">
         <f ca="1">C9*(LOG(C10/C21)/LOG(2))</f>
-        <v>54.199298874635083</v>
+        <v>55.283319439157466</v>
       </c>
       <c r="D26" t="s">
         <v>97</v>
@@ -44216,7 +44216,7 @@
       </c>
       <c r="C27" s="161">
         <f ca="1">C7+C26</f>
-        <v>43988.879531629267</v>
+        <v>43990.757182170637</v>
       </c>
       <c r="F27" t="s">
         <v>156</v>
@@ -44228,7 +44228,7 @@
       </c>
       <c r="C28" s="160">
         <f ca="1">C9*(LOG(C11/C21)/LOG(2))</f>
-        <v>34.942646006943704</v>
+        <v>35.641521225569086</v>
       </c>
       <c r="D28" t="s">
         <v>97</v>
@@ -44240,7 +44240,7 @@
       </c>
       <c r="C29" s="161">
         <f ca="1">C7+C28</f>
-        <v>43969.622878761576</v>
+        <v>43971.115383957047</v>
       </c>
       <c r="F29" t="s">
         <v>156</v>
@@ -44252,7 +44252,7 @@
       </c>
       <c r="C30" s="160">
         <f ca="1">C9*(LOG((C3*0.6)/C12)/LOG(2))</f>
-        <v>67.059147701941583</v>
+        <v>68.40037344946262</v>
       </c>
       <c r="D30" t="s">
         <v>97</v>
@@ -44264,7 +44264,7 @@
       </c>
       <c r="C31" s="161">
         <f ca="1">C7+C30</f>
-        <v>44001.739380456573</v>
+        <v>44003.874236180942</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
@@ -44273,7 +44273,7 @@
       </c>
       <c r="C34" s="150">
         <f ca="1">C7+30</f>
-        <v>43964.680232754632</v>
+        <v>43965.47386273148</v>
       </c>
       <c r="F34" t="s">
         <v>169</v>
@@ -44285,7 +44285,7 @@
       </c>
       <c r="C35" s="77">
         <f ca="1">C6*(2^((C34-C7)/C9))</f>
-        <v>483845.73840334476</v>
+        <v>446000.51108772145</v>
       </c>
       <c r="F35" t="s">
         <v>141</v>
@@ -44297,7 +44297,7 @@
       </c>
       <c r="C36" s="77">
         <f ca="1">C35/Projections!B6</f>
-        <v>4937201.4122790275</v>
+        <v>4551025.6233440964</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
@@ -44306,7 +44306,7 @@
       </c>
       <c r="C37" s="77">
         <f ca="1">C35*Projections!B10</f>
-        <v>391915.04810670926</v>
+        <v>361260.41398105439</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
@@ -44315,7 +44315,7 @@
       </c>
       <c r="C38" s="77">
         <f ca="1">C35*Projections!B11</f>
-        <v>67738.403376468268</v>
+        <v>62440.071552281006</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
@@ -44324,7 +44324,7 @@
       </c>
       <c r="C39" s="77">
         <f ca="1">C35*Projections!B12</f>
-        <v>24192.28692016724</v>
+        <v>22300.025554386073</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
@@ -44333,7 +44333,7 @@
       </c>
       <c r="C40" s="60">
         <f ca="1">C35*Projections!B13</f>
-        <v>14999.217890503687</v>
+        <v>13826.015843719364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
US deaths after 6 months from first US death
</commit_message>
<xml_diff>
--- a/Indian COVID-19 Infection Projections.xlsx
+++ b/Indian COVID-19 Infection Projections.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python\Aus COVID-19 Projections\Aus-COVID-19-Projections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0C6E1D-B857-4A1E-894B-333AB2A2D7D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84E47A6-B01B-46CA-B06E-67F49FC06FF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{744C986A-0D24-487A-A5C2-8E2494A78887}"/>
+    <workbookView xWindow="240" yWindow="0" windowWidth="37605" windowHeight="21000" activeTab="1" xr2:uid="{744C986A-0D24-487A-A5C2-8E2494A78887}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="4" r:id="rId1"/>
@@ -1890,46 +1890,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44019.868929861113</c:v>
+                  <c:v>44033.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44022.868929861113</c:v>
+                  <c:v>44036.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44025.868929861113</c:v>
+                  <c:v>44039.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44028.868929861113</c:v>
+                  <c:v>44042.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44031.868929861113</c:v>
+                  <c:v>44045.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44034.868929861113</c:v>
+                  <c:v>44048.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44037.868929861113</c:v>
+                  <c:v>44051.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44040.868929861113</c:v>
+                  <c:v>44054.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44043.868929861113</c:v>
+                  <c:v>44057.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44046.868929861113</c:v>
+                  <c:v>44060.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44049.868929861113</c:v>
+                  <c:v>44063.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44052.868929861113</c:v>
+                  <c:v>44066.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44055.868929861113</c:v>
+                  <c:v>44069.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44058.868929861113</c:v>
+                  <c:v>44072.627557754633</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2039,46 +2039,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44019.868929861113</c:v>
+                  <c:v>44033.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44022.868929861113</c:v>
+                  <c:v>44036.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44025.868929861113</c:v>
+                  <c:v>44039.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44028.868929861113</c:v>
+                  <c:v>44042.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44031.868929861113</c:v>
+                  <c:v>44045.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44034.868929861113</c:v>
+                  <c:v>44048.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44037.868929861113</c:v>
+                  <c:v>44051.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44040.868929861113</c:v>
+                  <c:v>44054.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44043.868929861113</c:v>
+                  <c:v>44057.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44046.868929861113</c:v>
+                  <c:v>44060.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44049.868929861113</c:v>
+                  <c:v>44063.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44052.868929861113</c:v>
+                  <c:v>44066.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44055.868929861113</c:v>
+                  <c:v>44069.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44058.868929861113</c:v>
+                  <c:v>44072.627557754633</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2188,46 +2188,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44019.868929861113</c:v>
+                  <c:v>44033.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44022.868929861113</c:v>
+                  <c:v>44036.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44025.868929861113</c:v>
+                  <c:v>44039.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44028.868929861113</c:v>
+                  <c:v>44042.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44031.868929861113</c:v>
+                  <c:v>44045.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44034.868929861113</c:v>
+                  <c:v>44048.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44037.868929861113</c:v>
+                  <c:v>44051.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44040.868929861113</c:v>
+                  <c:v>44054.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44043.868929861113</c:v>
+                  <c:v>44057.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44046.868929861113</c:v>
+                  <c:v>44060.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44049.868929861113</c:v>
+                  <c:v>44063.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44052.868929861113</c:v>
+                  <c:v>44066.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44055.868929861113</c:v>
+                  <c:v>44069.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44058.868929861113</c:v>
+                  <c:v>44072.627557754633</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2655,7 +2655,7 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2828,7 +2828,7 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3282,7 +3282,7 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3455,7 +3455,7 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3523,6 +3523,9 @@
                 </c:pt>
                 <c:pt idx="16" formatCode="#,##0">
                   <c:v>45578</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="#,##0">
+                  <c:v>63657</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3911,19 +3914,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3993,19 +3996,19 @@
                   <c:v>613826.46830447321</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1130712.3383375546</c:v>
+                  <c:v>2160340.3143666848</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2076477.4155147364</c:v>
+                  <c:v>3525960.1257974552</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3946445.6579263145</c:v>
+                  <c:v>6186238.171291858</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7574477.5277785007</c:v>
+                  <c:v>11207425.41127911</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>14643400.233504599</c:v>
+                  <c:v>20747040.567050006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4108,19 +4111,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4190,19 +4193,19 @@
                   <c:v>494481.7332995428</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>892701.81554373458</c:v>
+                  <c:v>1699346.4315334931</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1610551.1783329831</c:v>
+                  <c:v>2415019.0421491833</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3024877.0765085318</c:v>
+                  <c:v>4270209.9722007131</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5741276.6030261926</c:v>
+                  <c:v>7607305.1634356929</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>10993761.175946385</c:v>
+                  <c:v>13893256.798386922</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4305,19 +4308,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4387,19 +4390,19 @@
                   <c:v>93560.484304590718</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>179837.69459841074</c:v>
+                  <c:v>343598.10936079785</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>341429.59844683058</c:v>
+                  <c:v>593181.32683140342</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>665664.84653128218</c:v>
+                  <c:v>1083049.3480503368</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1304199.104616927</c:v>
+                  <c:v>2022085.1557456085</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2564504.8288418073</c:v>
+                  <c:v>3832389.553287704</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4502,19 +4505,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4584,19 +4587,19 @@
                   <c:v>45050.526671597006</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>86277.210293820026</c:v>
+                  <c:v>154788.21714627522</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>161591.90384841984</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>324235.2480844516</c:v>
+                  <c:v>28638.430511685787</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>638534.2580856448</c:v>
+                  <c:v>193088.2064832591</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1260305.7242248803</c:v>
+                  <c:v>547223.30781822046</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4699,19 +4702,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5178,19 +5181,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5377,19 +5380,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5576,19 +5579,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5776,19 +5779,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5976,19 +5979,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6175,19 +6178,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6372,19 +6375,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6572,19 +6575,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6771,19 +6774,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7250,19 +7253,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7449,19 +7452,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7648,19 +7651,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7848,19 +7851,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8045,19 +8048,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8244,19 +8247,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8441,19 +8444,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8638,19 +8641,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8837,19 +8840,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9316,19 +9319,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9515,19 +9518,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9714,19 +9717,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9911,19 +9914,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10110,19 +10113,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10307,19 +10310,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10786,19 +10789,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10985,19 +10988,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11182,19 +11185,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11381,19 +11384,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11578,19 +11581,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12052,7 +12055,7 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12225,7 +12228,7 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12680,7 +12683,7 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12853,7 +12856,7 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12921,6 +12924,9 @@
                 </c:pt>
                 <c:pt idx="16" formatCode="#,##0">
                   <c:v>45578</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="#,##0">
+                  <c:v>63657</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13249,46 +13255,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44019.868929861113</c:v>
+                  <c:v>44033.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44022.868929861113</c:v>
+                  <c:v>44036.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44025.868929861113</c:v>
+                  <c:v>44039.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44028.868929861113</c:v>
+                  <c:v>44042.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44031.868929861113</c:v>
+                  <c:v>44045.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44034.868929861113</c:v>
+                  <c:v>44048.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44037.868929861113</c:v>
+                  <c:v>44051.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44040.868929861113</c:v>
+                  <c:v>44054.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44043.868929861113</c:v>
+                  <c:v>44057.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44046.868929861113</c:v>
+                  <c:v>44060.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44049.868929861113</c:v>
+                  <c:v>44063.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44052.868929861113</c:v>
+                  <c:v>44066.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44055.868929861113</c:v>
+                  <c:v>44069.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44058.868929861113</c:v>
+                  <c:v>44072.627557754633</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13389,46 +13395,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44019.868929861113</c:v>
+                  <c:v>44033.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44022.868929861113</c:v>
+                  <c:v>44036.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44025.868929861113</c:v>
+                  <c:v>44039.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44028.868929861113</c:v>
+                  <c:v>44042.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44031.868929861113</c:v>
+                  <c:v>44045.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44034.868929861113</c:v>
+                  <c:v>44048.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44037.868929861113</c:v>
+                  <c:v>44051.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44040.868929861113</c:v>
+                  <c:v>44054.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44043.868929861113</c:v>
+                  <c:v>44057.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44046.868929861113</c:v>
+                  <c:v>44060.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44049.868929861113</c:v>
+                  <c:v>44063.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44052.868929861113</c:v>
+                  <c:v>44066.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44055.868929861113</c:v>
+                  <c:v>44069.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44058.868929861113</c:v>
+                  <c:v>44072.627557754633</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13532,46 +13538,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44019.868929861113</c:v>
+                  <c:v>44033.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44022.868929861113</c:v>
+                  <c:v>44036.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44025.868929861113</c:v>
+                  <c:v>44039.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44028.868929861113</c:v>
+                  <c:v>44042.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44031.868929861113</c:v>
+                  <c:v>44045.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44034.868929861113</c:v>
+                  <c:v>44048.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44037.868929861113</c:v>
+                  <c:v>44051.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44040.868929861113</c:v>
+                  <c:v>44054.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44043.868929861113</c:v>
+                  <c:v>44057.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44046.868929861113</c:v>
+                  <c:v>44060.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44049.868929861113</c:v>
+                  <c:v>44063.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44052.868929861113</c:v>
+                  <c:v>44066.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44055.868929861113</c:v>
+                  <c:v>44069.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44058.868929861113</c:v>
+                  <c:v>44072.627557754633</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13669,46 +13675,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44019.868929861113</c:v>
+                  <c:v>44033.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44022.868929861113</c:v>
+                  <c:v>44036.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44025.868929861113</c:v>
+                  <c:v>44039.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44028.868929861113</c:v>
+                  <c:v>44042.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44031.868929861113</c:v>
+                  <c:v>44045.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44034.868929861113</c:v>
+                  <c:v>44048.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44037.868929861113</c:v>
+                  <c:v>44051.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44040.868929861113</c:v>
+                  <c:v>44054.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44043.868929861113</c:v>
+                  <c:v>44057.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44046.868929861113</c:v>
+                  <c:v>44060.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44049.868929861113</c:v>
+                  <c:v>44063.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44052.868929861113</c:v>
+                  <c:v>44066.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44055.868929861113</c:v>
+                  <c:v>44069.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44058.868929861113</c:v>
+                  <c:v>44072.627557754633</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14076,46 +14082,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44019.868929861113</c:v>
+                  <c:v>44033.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44022.868929861113</c:v>
+                  <c:v>44036.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44025.868929861113</c:v>
+                  <c:v>44039.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44028.868929861113</c:v>
+                  <c:v>44042.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44031.868929861113</c:v>
+                  <c:v>44045.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44034.868929861113</c:v>
+                  <c:v>44048.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44037.868929861113</c:v>
+                  <c:v>44051.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44040.868929861113</c:v>
+                  <c:v>44054.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44043.868929861113</c:v>
+                  <c:v>44057.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44046.868929861113</c:v>
+                  <c:v>44060.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44049.868929861113</c:v>
+                  <c:v>44063.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44052.868929861113</c:v>
+                  <c:v>44066.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44055.868929861113</c:v>
+                  <c:v>44069.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44058.868929861113</c:v>
+                  <c:v>44072.627557754633</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14225,46 +14231,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44019.868929861113</c:v>
+                  <c:v>44033.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44022.868929861113</c:v>
+                  <c:v>44036.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44025.868929861113</c:v>
+                  <c:v>44039.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44028.868929861113</c:v>
+                  <c:v>44042.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44031.868929861113</c:v>
+                  <c:v>44045.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44034.868929861113</c:v>
+                  <c:v>44048.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44037.868929861113</c:v>
+                  <c:v>44051.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44040.868929861113</c:v>
+                  <c:v>44054.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44043.868929861113</c:v>
+                  <c:v>44057.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44046.868929861113</c:v>
+                  <c:v>44060.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44049.868929861113</c:v>
+                  <c:v>44063.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44052.868929861113</c:v>
+                  <c:v>44066.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44055.868929861113</c:v>
+                  <c:v>44069.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44058.868929861113</c:v>
+                  <c:v>44072.627557754633</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14374,46 +14380,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44019.868929861113</c:v>
+                  <c:v>44033.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44022.868929861113</c:v>
+                  <c:v>44036.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44025.868929861113</c:v>
+                  <c:v>44039.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44028.868929861113</c:v>
+                  <c:v>44042.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44031.868929861113</c:v>
+                  <c:v>44045.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44034.868929861113</c:v>
+                  <c:v>44048.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44037.868929861113</c:v>
+                  <c:v>44051.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44040.868929861113</c:v>
+                  <c:v>44054.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44043.868929861113</c:v>
+                  <c:v>44057.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44046.868929861113</c:v>
+                  <c:v>44060.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44049.868929861113</c:v>
+                  <c:v>44063.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44052.868929861113</c:v>
+                  <c:v>44066.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44055.868929861113</c:v>
+                  <c:v>44069.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44058.868929861113</c:v>
+                  <c:v>44072.627557754633</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14791,46 +14797,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44019.868929861113</c:v>
+                  <c:v>44033.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44022.868929861113</c:v>
+                  <c:v>44036.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44025.868929861113</c:v>
+                  <c:v>44039.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44028.868929861113</c:v>
+                  <c:v>44042.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44031.868929861113</c:v>
+                  <c:v>44045.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44034.868929861113</c:v>
+                  <c:v>44048.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44037.868929861113</c:v>
+                  <c:v>44051.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44040.868929861113</c:v>
+                  <c:v>44054.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44043.868929861113</c:v>
+                  <c:v>44057.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44046.868929861113</c:v>
+                  <c:v>44060.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44049.868929861113</c:v>
+                  <c:v>44063.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44052.868929861113</c:v>
+                  <c:v>44066.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44055.868929861113</c:v>
+                  <c:v>44069.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44058.868929861113</c:v>
+                  <c:v>44072.627557754633</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14931,46 +14937,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44019.868929861113</c:v>
+                  <c:v>44033.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44022.868929861113</c:v>
+                  <c:v>44036.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44025.868929861113</c:v>
+                  <c:v>44039.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44028.868929861113</c:v>
+                  <c:v>44042.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44031.868929861113</c:v>
+                  <c:v>44045.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44034.868929861113</c:v>
+                  <c:v>44048.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44037.868929861113</c:v>
+                  <c:v>44051.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44040.868929861113</c:v>
+                  <c:v>44054.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44043.868929861113</c:v>
+                  <c:v>44057.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44046.868929861113</c:v>
+                  <c:v>44060.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44049.868929861113</c:v>
+                  <c:v>44063.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44052.868929861113</c:v>
+                  <c:v>44066.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44055.868929861113</c:v>
+                  <c:v>44069.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44058.868929861113</c:v>
+                  <c:v>44072.627557754633</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15074,46 +15080,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44019.868929861113</c:v>
+                  <c:v>44033.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44022.868929861113</c:v>
+                  <c:v>44036.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44025.868929861113</c:v>
+                  <c:v>44039.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44028.868929861113</c:v>
+                  <c:v>44042.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44031.868929861113</c:v>
+                  <c:v>44045.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44034.868929861113</c:v>
+                  <c:v>44048.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44037.868929861113</c:v>
+                  <c:v>44051.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44040.868929861113</c:v>
+                  <c:v>44054.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44043.868929861113</c:v>
+                  <c:v>44057.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44046.868929861113</c:v>
+                  <c:v>44060.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44049.868929861113</c:v>
+                  <c:v>44063.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44052.868929861113</c:v>
+                  <c:v>44066.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44055.868929861113</c:v>
+                  <c:v>44069.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44058.868929861113</c:v>
+                  <c:v>44072.627557754633</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15211,46 +15217,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44019.868929861113</c:v>
+                  <c:v>44033.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44022.868929861113</c:v>
+                  <c:v>44036.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44025.868929861113</c:v>
+                  <c:v>44039.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44028.868929861113</c:v>
+                  <c:v>44042.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44031.868929861113</c:v>
+                  <c:v>44045.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44034.868929861113</c:v>
+                  <c:v>44048.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44037.868929861113</c:v>
+                  <c:v>44051.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44040.868929861113</c:v>
+                  <c:v>44054.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44043.868929861113</c:v>
+                  <c:v>44057.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44046.868929861113</c:v>
+                  <c:v>44060.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44049.868929861113</c:v>
+                  <c:v>44063.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44052.868929861113</c:v>
+                  <c:v>44066.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44055.868929861113</c:v>
+                  <c:v>44069.627557754633</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44058.868929861113</c:v>
+                  <c:v>44072.627557754633</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15680,19 +15686,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15762,19 +15768,19 @@
                   <c:v>613826.46830447321</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1130712.3383375546</c:v>
+                  <c:v>2160340.3143666848</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2076477.4155147364</c:v>
+                  <c:v>3525960.1257974552</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3946445.6579263145</c:v>
+                  <c:v>6186238.171291858</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7574477.5277785007</c:v>
+                  <c:v>11207425.41127911</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>14643400.233504599</c:v>
+                  <c:v>20747040.567050006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15877,19 +15883,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15959,19 +15965,19 @@
                   <c:v>494481.7332995428</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>892701.81554373458</c:v>
+                  <c:v>1699346.4315334931</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1610551.1783329831</c:v>
+                  <c:v>2415019.0421491833</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3024877.0765085318</c:v>
+                  <c:v>4270209.9722007131</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5741276.6030261926</c:v>
+                  <c:v>7607305.1634356929</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>10993761.175946385</c:v>
+                  <c:v>13893256.798386922</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16074,19 +16080,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16156,19 +16162,19 @@
                   <c:v>93560.484304590718</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>179837.69459841074</c:v>
+                  <c:v>343598.10936079785</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>341429.59844683058</c:v>
+                  <c:v>593181.32683140342</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>665664.84653128218</c:v>
+                  <c:v>1083049.3480503368</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1304199.104616927</c:v>
+                  <c:v>2022085.1557456085</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2564504.8288418073</c:v>
+                  <c:v>3832389.553287704</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16271,19 +16277,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16353,19 +16359,19 @@
                   <c:v>45050.526671597006</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>86277.210293820026</c:v>
+                  <c:v>154788.21714627522</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>161591.90384841984</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>324235.2480844516</c:v>
+                  <c:v>28638.430511685787</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>638534.2580856448</c:v>
+                  <c:v>193088.2064832591</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1260305.7242248803</c:v>
+                  <c:v>547223.30781822046</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16468,19 +16474,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16946,19 +16952,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17145,19 +17151,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17344,19 +17350,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17544,19 +17550,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17744,19 +17750,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17943,19 +17949,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -18140,19 +18146,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -18340,19 +18346,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -18539,19 +18545,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -19017,19 +19023,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -19216,19 +19222,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -19415,19 +19421,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -19615,19 +19621,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -19812,19 +19818,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -20011,19 +20017,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -20208,19 +20214,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -20405,19 +20411,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -20604,19 +20610,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -21082,19 +21088,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -21281,19 +21287,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -21480,19 +21486,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -21677,19 +21683,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -21876,19 +21882,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -22073,19 +22079,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -22551,19 +22557,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -22750,19 +22756,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -22947,19 +22953,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -23146,19 +23152,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -23343,19 +23349,19 @@
                   <c:v>44050</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44071</c:v>
+                  <c:v>44080</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44092</c:v>
+                  <c:v>44110</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44113</c:v>
+                  <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44134</c:v>
+                  <c:v>44170</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44155</c:v>
+                  <c:v>44200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -35402,167 +35408,167 @@
       </c>
       <c r="B26" s="83">
         <f t="shared" ref="B26:G26" ca="1" si="0">C26-1</f>
-        <v>44019.868929861113</v>
+        <v>44033.627557754633</v>
       </c>
       <c r="C26" s="84">
         <f t="shared" ca="1" si="0"/>
-        <v>44020.868929861113</v>
+        <v>44034.627557754633</v>
       </c>
       <c r="D26" s="84">
         <f t="shared" ca="1" si="0"/>
-        <v>44021.868929861113</v>
+        <v>44035.627557754633</v>
       </c>
       <c r="E26" s="84">
         <f t="shared" ca="1" si="0"/>
-        <v>44022.868929861113</v>
+        <v>44036.627557754633</v>
       </c>
       <c r="F26" s="84">
         <f t="shared" ca="1" si="0"/>
-        <v>44023.868929861113</v>
+        <v>44037.627557754633</v>
       </c>
       <c r="G26" s="85">
         <f t="shared" ca="1" si="0"/>
-        <v>44024.868929861113</v>
+        <v>44038.627557754633</v>
       </c>
       <c r="H26" s="84">
         <f t="shared" ref="H26:U26" ca="1" si="1">I26-1</f>
-        <v>44025.868929861113</v>
+        <v>44039.627557754633</v>
       </c>
       <c r="I26" s="84">
         <f t="shared" ca="1" si="1"/>
-        <v>44026.868929861113</v>
+        <v>44040.627557754633</v>
       </c>
       <c r="J26" s="84">
         <f t="shared" ca="1" si="1"/>
-        <v>44027.868929861113</v>
+        <v>44041.627557754633</v>
       </c>
       <c r="K26" s="84">
         <f t="shared" ca="1" si="1"/>
-        <v>44028.868929861113</v>
+        <v>44042.627557754633</v>
       </c>
       <c r="L26" s="84">
         <f t="shared" ca="1" si="1"/>
-        <v>44029.868929861113</v>
+        <v>44043.627557754633</v>
       </c>
       <c r="M26" s="84">
         <f t="shared" ca="1" si="1"/>
-        <v>44030.868929861113</v>
+        <v>44044.627557754633</v>
       </c>
       <c r="N26" s="85">
         <f t="shared" ca="1" si="1"/>
-        <v>44031.868929861113</v>
+        <v>44045.627557754633</v>
       </c>
       <c r="O26" s="83">
         <f t="shared" ca="1" si="1"/>
-        <v>44032.868929861113</v>
+        <v>44046.627557754633</v>
       </c>
       <c r="P26" s="84">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.868929861113</v>
+        <v>44047.627557754633</v>
       </c>
       <c r="Q26" s="84">
         <f t="shared" ca="1" si="1"/>
-        <v>44034.868929861113</v>
+        <v>44048.627557754633</v>
       </c>
       <c r="R26" s="84">
         <f t="shared" ca="1" si="1"/>
-        <v>44035.868929861113</v>
+        <v>44049.627557754633</v>
       </c>
       <c r="S26" s="84">
         <f t="shared" ca="1" si="1"/>
-        <v>44036.868929861113</v>
+        <v>44050.627557754633</v>
       </c>
       <c r="T26" s="84">
         <f t="shared" ca="1" si="1"/>
-        <v>44037.868929861113</v>
+        <v>44051.627557754633</v>
       </c>
       <c r="U26" s="85">
         <f t="shared" ca="1" si="1"/>
-        <v>44038.868929861113</v>
+        <v>44052.627557754633</v>
       </c>
       <c r="V26" s="83">
         <f t="shared" ref="V26:AN26" ca="1" si="2">W26-1</f>
-        <v>44039.868929861113</v>
+        <v>44053.627557754633</v>
       </c>
       <c r="W26" s="84">
         <f t="shared" ca="1" si="2"/>
-        <v>44040.868929861113</v>
+        <v>44054.627557754633</v>
       </c>
       <c r="X26" s="84">
         <f t="shared" ca="1" si="2"/>
-        <v>44041.868929861113</v>
+        <v>44055.627557754633</v>
       </c>
       <c r="Y26" s="84">
         <f t="shared" ca="1" si="2"/>
-        <v>44042.868929861113</v>
+        <v>44056.627557754633</v>
       </c>
       <c r="Z26" s="84">
         <f t="shared" ca="1" si="2"/>
-        <v>44043.868929861113</v>
+        <v>44057.627557754633</v>
       </c>
       <c r="AA26" s="84">
         <f t="shared" ca="1" si="2"/>
-        <v>44044.868929861113</v>
+        <v>44058.627557754633</v>
       </c>
       <c r="AB26" s="85">
         <f t="shared" ca="1" si="2"/>
-        <v>44045.868929861113</v>
+        <v>44059.627557754633</v>
       </c>
       <c r="AC26" s="83">
         <f t="shared" ca="1" si="2"/>
-        <v>44046.868929861113</v>
+        <v>44060.627557754633</v>
       </c>
       <c r="AD26" s="84">
         <f t="shared" ca="1" si="2"/>
-        <v>44047.868929861113</v>
+        <v>44061.627557754633</v>
       </c>
       <c r="AE26" s="84">
         <f t="shared" ca="1" si="2"/>
-        <v>44048.868929861113</v>
+        <v>44062.627557754633</v>
       </c>
       <c r="AF26" s="84">
         <f t="shared" ca="1" si="2"/>
-        <v>44049.868929861113</v>
+        <v>44063.627557754633</v>
       </c>
       <c r="AG26" s="84">
         <f t="shared" ca="1" si="2"/>
-        <v>44050.868929861113</v>
+        <v>44064.627557754633</v>
       </c>
       <c r="AH26" s="84">
         <f t="shared" ca="1" si="2"/>
-        <v>44051.868929861113</v>
+        <v>44065.627557754633</v>
       </c>
       <c r="AI26" s="85">
         <f t="shared" ca="1" si="2"/>
-        <v>44052.868929861113</v>
+        <v>44066.627557754633</v>
       </c>
       <c r="AJ26" s="83">
         <f t="shared" ca="1" si="2"/>
-        <v>44053.868929861113</v>
+        <v>44067.627557754633</v>
       </c>
       <c r="AK26" s="84">
         <f t="shared" ca="1" si="2"/>
-        <v>44054.868929861113</v>
+        <v>44068.627557754633</v>
       </c>
       <c r="AL26" s="84">
         <f t="shared" ca="1" si="2"/>
-        <v>44055.868929861113</v>
+        <v>44069.627557754633</v>
       </c>
       <c r="AM26" s="84">
         <f t="shared" ca="1" si="2"/>
-        <v>44056.868929861113</v>
+        <v>44070.627557754633</v>
       </c>
       <c r="AN26" s="84">
         <f t="shared" ca="1" si="2"/>
-        <v>44057.868929861113</v>
+        <v>44071.627557754633</v>
       </c>
       <c r="AO26" s="84">
         <f ca="1">AP26-1</f>
-        <v>44058.868929861113</v>
+        <v>44072.627557754633</v>
       </c>
       <c r="AP26" s="105">
         <f ca="1">NOW()</f>
-        <v>44059.868929861113</v>
+        <v>44073.627557754633</v>
       </c>
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.25">
@@ -36080,8 +36086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9BB0FAD-39ED-4D53-8BC6-75164ED434B0}">
   <dimension ref="A1:AR104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="V18" sqref="V18"/>
+    <sheetView tabSelected="1" topLeftCell="L20" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AL14" sqref="AL14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36705,7 +36711,7 @@
       <c r="C25" s="2"/>
       <c r="D25" s="268">
         <f>(AI28-N28)/(LOG(AI29/N29)/LOG(2))</f>
-        <v>12.380952380952381</v>
+        <v>14.523809523809524</v>
       </c>
       <c r="E25" s="164"/>
       <c r="Q25" s="16"/>
@@ -36784,7 +36790,9 @@
       <c r="J27" s="178">
         <v>44008</v>
       </c>
-      <c r="K27" s="178"/>
+      <c r="K27" s="178">
+        <v>44050</v>
+      </c>
       <c r="L27" s="178"/>
       <c r="M27" s="178"/>
       <c r="O27" s="127" t="s">
@@ -36841,7 +36849,9 @@
       <c r="J28" s="206">
         <v>21</v>
       </c>
-      <c r="K28" s="206"/>
+      <c r="K28" s="206">
+        <v>30</v>
+      </c>
       <c r="L28" s="206"/>
       <c r="M28" s="206"/>
       <c r="N28" s="290">
@@ -36913,47 +36923,47 @@
       </c>
       <c r="AE28" s="216">
         <f t="shared" si="0"/>
-        <v>44071</v>
+        <v>44080</v>
       </c>
       <c r="AF28" s="216">
         <f t="shared" si="0"/>
-        <v>44092</v>
+        <v>44110</v>
       </c>
       <c r="AG28" s="216">
         <f t="shared" si="0"/>
-        <v>44113</v>
+        <v>44140</v>
       </c>
       <c r="AH28" s="216">
         <f t="shared" ref="AH28" si="1">AG28+HLOOKUP(AG28+1, $B$27:$M$28,2,TRUE)</f>
-        <v>44134</v>
+        <v>44170</v>
       </c>
       <c r="AI28" s="223">
         <f t="shared" ref="AI28" si="2">AH28+HLOOKUP(AH28+1, $B$27:$M$28,2,TRUE)</f>
-        <v>44155</v>
+        <v>44200</v>
       </c>
       <c r="AJ28" s="216">
         <f>AI28+HLOOKUP(AI28+1, $B$27:$M$28,2,TRUE)</f>
-        <v>44176</v>
+        <v>44230</v>
       </c>
       <c r="AK28" s="216">
         <f>AJ28+HLOOKUP(AJ28+1, $B$27:$M$28,2,TRUE)</f>
-        <v>44197</v>
+        <v>44260</v>
       </c>
       <c r="AL28" s="216">
         <f>AK28+HLOOKUP(AK28+1, $B$27:$M$28,2,TRUE)</f>
-        <v>44218</v>
+        <v>44290</v>
       </c>
       <c r="AM28" s="223">
         <f>AK28+HLOOKUP(AK28+1, $B$27:$M$28,2,TRUE)</f>
-        <v>44218</v>
+        <v>44290</v>
       </c>
       <c r="AN28" s="223">
         <f>AM28+HLOOKUP(AM28+1, $B$27:$M$28,2,TRUE)</f>
-        <v>44239</v>
+        <v>44320</v>
       </c>
       <c r="AO28" s="235">
         <f>AN28+(7*8)</f>
-        <v>44295</v>
+        <v>44376</v>
       </c>
       <c r="AP28" s="67"/>
       <c r="AQ28" s="67"/>
@@ -37308,43 +37318,43 @@
       </c>
       <c r="AE31" s="270">
         <f t="shared" si="9"/>
-        <v>851058.3404073352</v>
+        <v>128436.2249522857</v>
       </c>
       <c r="AF31" s="270">
         <f t="shared" si="9"/>
-        <v>2015076.5733811799</v>
+        <v>0</v>
       </c>
       <c r="AG31" s="270">
         <f t="shared" si="9"/>
-        <v>4337231.3063286161</v>
+        <v>142520.88337020413</v>
       </c>
       <c r="AH31" s="270">
         <f t="shared" ref="AH31:AM31" si="10">MAX(AH29-(AH37-AH38)-(AH39-AH40)-(AH41-AH42),0)</f>
-        <v>9141108.7339221947</v>
+        <v>796802.80289423326</v>
       </c>
       <c r="AI31" s="270">
         <f t="shared" si="10"/>
-        <v>19037183.610587582</v>
+        <v>2312889.9858674323</v>
       </c>
       <c r="AJ31" s="270">
         <f t="shared" si="10"/>
-        <v>39320786.036446229</v>
+        <v>5690501.1763516515</v>
       </c>
       <c r="AK31" s="270">
         <f t="shared" si="10"/>
-        <v>80734077.627599984</v>
+        <v>13019180.633083928</v>
       </c>
       <c r="AL31" s="226">
         <f t="shared" ref="AL31" si="11">MAX(AL29-(AL37-AL38)-(AL39-AL40)-(AL41-AL42),0)</f>
-        <v>165030793.44225243</v>
+        <v>28635446.386399403</v>
       </c>
       <c r="AM31" s="186">
         <f t="shared" si="10"/>
-        <v>689318793.44225228</v>
+        <v>531904484.92311698</v>
       </c>
       <c r="AN31" s="185">
         <f t="shared" si="9"/>
-        <v>679780254.4150182</v>
+        <v>385156083.88442975</v>
       </c>
       <c r="AO31" s="230"/>
       <c r="AP31" s="45"/>
@@ -37437,43 +37447,43 @@
       </c>
       <c r="AE32" s="210">
         <f t="shared" si="12"/>
-        <v>3203775.0464986451</v>
+        <v>3884487.4224733245</v>
       </c>
       <c r="AF32" s="210">
         <f t="shared" si="12"/>
-        <v>6097794.8409955194</v>
+        <v>7903149.2624014225</v>
       </c>
       <c r="AG32" s="210">
         <f t="shared" si="12"/>
-        <v>11896539.670354778</v>
+        <v>15777538.31291279</v>
       </c>
       <c r="AH32" s="210">
         <f t="shared" si="12"/>
-        <v>23333998.73360404</v>
+        <v>31166438.539430331</v>
       </c>
       <c r="AI32" s="210">
         <f t="shared" si="12"/>
-        <v>45924968.78338097</v>
+        <v>61777636.866125993</v>
       </c>
       <c r="AJ32" s="210">
         <f>MAX(AJ29-AJ31-AJ44,0)</f>
-        <v>90622831.838863373</v>
+        <v>122723588.31845975</v>
       </c>
       <c r="AK32" s="210">
         <f>MAX(AK29-AK31-AK44,0)</f>
-        <v>179185043.25550291</v>
+        <v>244156025.93675405</v>
       </c>
       <c r="AL32" s="292">
         <f t="shared" ref="AL32:AM32" si="13">MAX(AL29-AL31-AL44,0)</f>
-        <v>354860977.53581798</v>
+        <v>486250715.53262228</v>
       </c>
       <c r="AM32" s="293">
         <f t="shared" si="13"/>
-        <v>354860977.5358181</v>
+        <v>507269676.99590468</v>
       </c>
       <c r="AN32" s="200">
         <f>MAX(AN29-AN31-AN44,0)</f>
-        <v>703674424.79707038</v>
+        <v>989047165.23541677</v>
       </c>
       <c r="AO32" s="231"/>
       <c r="AP32" s="25"/>
@@ -37977,23 +37987,23 @@
       </c>
       <c r="AI36" s="184">
         <f t="shared" si="24"/>
-        <v>112838212.46903951</v>
+        <v>144179200</v>
       </c>
       <c r="AJ36" s="184">
         <f t="shared" si="24"/>
-        <v>222487911.68971121</v>
+        <v>288358400</v>
       </c>
       <c r="AK36" s="184">
         <f t="shared" si="24"/>
-        <v>439622902.19296128</v>
+        <v>576716800</v>
       </c>
       <c r="AL36" s="227">
         <f t="shared" si="24"/>
-        <v>870132078.79113722</v>
+        <v>1153433600</v>
       </c>
       <c r="AM36" s="190">
         <f t="shared" si="24"/>
-        <v>870132078.79113722</v>
+        <v>1210522137.3076808</v>
       </c>
       <c r="AN36" s="189">
         <f t="shared" si="24"/>
@@ -38222,43 +38232,43 @@
       </c>
       <c r="AE38" s="191">
         <f t="shared" si="28"/>
-        <v>404389.34750574594</v>
+        <v>0</v>
       </c>
       <c r="AF38" s="191">
         <f t="shared" si="28"/>
-        <v>1104360.5051613441</v>
+        <v>0</v>
       </c>
       <c r="AG38" s="191">
         <f t="shared" si="28"/>
-        <v>2487269.4861932285</v>
+        <v>0</v>
       </c>
       <c r="AH38" s="191">
         <f t="shared" si="28"/>
-        <v>5414054.505205784</v>
+        <v>0</v>
       </c>
       <c r="AI38" s="191">
         <f t="shared" si="28"/>
-        <v>11539181.772762723</v>
+        <v>0</v>
       </c>
       <c r="AJ38" s="191">
         <f t="shared" si="28"/>
-        <v>24252316.150606334</v>
+        <v>0</v>
       </c>
       <c r="AK38" s="191">
         <f t="shared" si="28"/>
-        <v>50475480.556227893</v>
+        <v>0</v>
       </c>
       <c r="AL38" s="227">
         <f t="shared" si="28"/>
-        <v>104306469.17235404</v>
+        <v>0</v>
       </c>
       <c r="AM38" s="190">
         <f t="shared" si="28"/>
-        <v>528979749.17235404</v>
+        <v>403654318.53671753</v>
       </c>
       <c r="AN38" s="189">
         <f t="shared" si="28"/>
-        <v>492694506.60019159</v>
+        <v>258388327.3955977</v>
       </c>
       <c r="AO38" s="230"/>
       <c r="AP38" s="25"/>
@@ -38351,43 +38361,43 @@
       </c>
       <c r="AE39" s="198">
         <f t="shared" si="29"/>
-        <v>1130712.3383375546</v>
+        <v>2160340.3143666848</v>
       </c>
       <c r="AF39" s="198">
         <f t="shared" si="29"/>
-        <v>2076477.4155147364</v>
+        <v>3525960.1257974552</v>
       </c>
       <c r="AG39" s="198">
         <f t="shared" si="29"/>
-        <v>3946445.6579263145</v>
+        <v>6186238.171291858</v>
       </c>
       <c r="AH39" s="198">
         <f t="shared" si="29"/>
-        <v>7574477.5277785007</v>
+        <v>11207425.41127911</v>
       </c>
       <c r="AI39" s="198">
         <f t="shared" si="29"/>
-        <v>14643400.233504599</v>
+        <v>20747040.567050006</v>
       </c>
       <c r="AJ39" s="198">
         <f t="shared" si="29"/>
-        <v>28465078.188948456</v>
+        <v>38995302.803976551</v>
       </c>
       <c r="AK39" s="198">
         <f t="shared" si="29"/>
-        <v>55568690.677641883</v>
+        <v>74113884.460975721</v>
       </c>
       <c r="AL39" s="224">
         <f t="shared" si="29"/>
-        <v>108845357.51685539</v>
+        <v>142045262.54452562</v>
       </c>
       <c r="AM39" s="195">
         <f t="shared" si="29"/>
-        <v>108845357.51685539</v>
+        <v>142045262.54452562</v>
       </c>
       <c r="AN39" s="194">
         <f>($N$29*($B$22+$B$23))*(2^(((AN28 - 7) - $N$28)/AN54))</f>
-        <v>192382052.8753719</v>
+        <v>206014319.92070228</v>
       </c>
       <c r="AO39" s="230">
         <f>AO29*(B22+B23)</f>
@@ -38483,43 +38493,43 @@
       </c>
       <c r="AE40" s="184">
         <f t="shared" si="31"/>
-        <v>892701.81554373458</v>
+        <v>1699346.4315334931</v>
       </c>
       <c r="AF40" s="184">
         <f t="shared" si="31"/>
-        <v>1610551.1783329831</v>
+        <v>2415019.0421491833</v>
       </c>
       <c r="AG40" s="184">
         <f t="shared" si="31"/>
-        <v>3024877.0765085318</v>
+        <v>4270209.9722007131</v>
       </c>
       <c r="AH40" s="184">
         <f t="shared" si="31"/>
-        <v>5741276.6030261926</v>
+        <v>7607305.1634356929</v>
       </c>
       <c r="AI40" s="184">
         <f t="shared" si="31"/>
-        <v>10993761.175946385</v>
+        <v>13893256.798386922</v>
       </c>
       <c r="AJ40" s="184">
         <f t="shared" si="31"/>
-        <v>21194372.90363016</v>
+        <v>25822829.673938662</v>
       </c>
       <c r="AK40" s="184">
         <f t="shared" si="31"/>
-        <v>41076471.196507402</v>
+        <v>48618417.435336947</v>
       </c>
       <c r="AL40" s="227">
         <f t="shared" si="31"/>
-        <v>79946391.382048339</v>
+        <v>92433802.751330331</v>
       </c>
       <c r="AM40" s="190">
         <f t="shared" si="31"/>
-        <v>79946391.382048339</v>
+        <v>92433802.751330331</v>
       </c>
       <c r="AN40" s="189">
         <f t="shared" si="31"/>
-        <v>134733889.75363353</v>
+        <v>109074142.95533797</v>
       </c>
       <c r="AO40" s="232"/>
       <c r="AP40" s="45"/>
@@ -38612,43 +38622,43 @@
       </c>
       <c r="AE41" s="198">
         <f t="shared" si="32"/>
-        <v>179837.69459841074</v>
+        <v>343598.10936079785</v>
       </c>
       <c r="AF41" s="198">
         <f t="shared" si="32"/>
-        <v>341429.59844683058</v>
+        <v>593181.32683140342</v>
       </c>
       <c r="AG41" s="198">
         <f t="shared" si="32"/>
-        <v>665664.84653128218</v>
+        <v>1083049.3480503368</v>
       </c>
       <c r="AH41" s="198">
         <f t="shared" si="32"/>
-        <v>1304199.104616927</v>
+        <v>2022085.1557456085</v>
       </c>
       <c r="AI41" s="198">
         <f t="shared" si="32"/>
-        <v>2564504.8288418073</v>
+        <v>3832389.553287704</v>
       </c>
       <c r="AJ41" s="198">
         <f t="shared" si="32"/>
-        <v>5056543.4474934367</v>
+        <v>7340661.9177636048</v>
       </c>
       <c r="AK41" s="198">
         <f t="shared" si="32"/>
-        <v>9991429.5952945743</v>
+        <v>14169730.469394304</v>
       </c>
       <c r="AL41" s="224">
         <f t="shared" si="32"/>
-        <v>19775729.063434936</v>
+        <v>27511866.756992746</v>
       </c>
       <c r="AM41" s="195">
         <f t="shared" si="32"/>
-        <v>19775729.063434936</v>
+        <v>27511866.756992746</v>
       </c>
       <c r="AN41" s="194">
         <f t="shared" si="32"/>
-        <v>39194558.851840027</v>
+        <v>53657903.247185335</v>
       </c>
       <c r="AO41" s="230">
         <f>AO29*B23</f>
@@ -38744,43 +38754,43 @@
       </c>
       <c r="AE42" s="191">
         <f t="shared" si="34"/>
-        <v>86277.210293820026</v>
+        <v>154788.21714627522</v>
       </c>
       <c r="AF42" s="191">
         <f t="shared" si="34"/>
-        <v>161591.90384841984</v>
+        <v>0</v>
       </c>
       <c r="AG42" s="191">
         <f t="shared" si="34"/>
-        <v>324235.2480844516</v>
+        <v>28638.430511685787</v>
       </c>
       <c r="AH42" s="191">
         <f t="shared" si="34"/>
-        <v>638534.2580856448</v>
+        <v>193088.2064832591</v>
       </c>
       <c r="AI42" s="191">
         <f t="shared" si="34"/>
-        <v>1260305.7242248803</v>
+        <v>547223.30781822046</v>
       </c>
       <c r="AJ42" s="191">
         <f t="shared" si="34"/>
-        <v>2492038.6186516294</v>
+        <v>1299956.2241531452</v>
       </c>
       <c r="AK42" s="191">
         <f t="shared" si="34"/>
-        <v>4934886.1478011375</v>
+        <v>2877018.1281170063</v>
       </c>
       <c r="AL42" s="227">
         <f t="shared" si="34"/>
-        <v>9784299.4681403618</v>
+        <v>6144052.9365874417</v>
       </c>
       <c r="AM42" s="190">
         <f t="shared" si="34"/>
-        <v>9784299.4681403618</v>
+        <v>6144052.9365874417</v>
       </c>
       <c r="AN42" s="189">
         <f t="shared" si="34"/>
-        <v>19418829.788405091</v>
+        <v>12856196.701381736</v>
       </c>
       <c r="AO42" s="230"/>
       <c r="AP42" s="45"/>
@@ -38981,47 +38991,47 @@
       </c>
       <c r="AE44" s="196">
         <f t="shared" si="38"/>
-        <v>41166.613094019915</v>
+        <v>83076.352574389966</v>
       </c>
       <c r="AF44" s="196">
         <f t="shared" si="38"/>
-        <v>79128.585623300736</v>
+        <v>288850.73759857769</v>
       </c>
       <c r="AG44" s="196">
         <f t="shared" si="38"/>
-        <v>150229.02331660545</v>
+        <v>463940.80371700646</v>
       </c>
       <c r="AH44" s="196">
         <f t="shared" si="38"/>
-        <v>292892.53247376415</v>
+        <v>804758.65767543379</v>
       </c>
       <c r="AI44" s="196">
         <f t="shared" si="38"/>
-        <v>573847.60603144788</v>
+        <v>1445473.1480065729</v>
       </c>
       <c r="AJ44" s="196">
         <f t="shared" si="38"/>
-        <v>1128382.1246903951</v>
+        <v>2657910.505188602</v>
       </c>
       <c r="AK44" s="196">
         <f t="shared" si="38"/>
-        <v>2224879.1168971122</v>
+        <v>4968793.4301620107</v>
       </c>
       <c r="AL44" s="227">
         <f t="shared" si="38"/>
-        <v>4396229.0219296124</v>
+        <v>9401838.080978334</v>
       </c>
       <c r="AM44" s="190">
         <f t="shared" si="38"/>
-        <v>4396229.0219296124</v>
+        <v>9401838.080978334</v>
       </c>
       <c r="AN44" s="189">
         <f t="shared" si="38"/>
-        <v>8701320.7879113723</v>
+        <v>17952750.880153582</v>
       </c>
       <c r="AO44" s="233">
         <f>($N$29*$B$24)*(2^(((AO28 - 35) - $N$28)/AO54))</f>
-        <v>6807925.1070761289</v>
+        <v>8830414.1208375618</v>
       </c>
       <c r="AP44" s="45"/>
       <c r="AQ44" s="45"/>
@@ -39113,15 +39123,15 @@
       </c>
       <c r="AE45" s="140">
         <f t="shared" si="39"/>
-        <v>44064</v>
+        <v>44073</v>
       </c>
       <c r="AF45" s="140">
         <f t="shared" si="39"/>
-        <v>44085</v>
+        <v>44103</v>
       </c>
       <c r="AG45" s="140">
         <f t="shared" si="39"/>
-        <v>44106</v>
+        <v>44133</v>
       </c>
       <c r="AH45" s="140"/>
       <c r="AI45" s="140"/>
@@ -39131,7 +39141,7 @@
       <c r="AM45" s="140"/>
       <c r="AN45" s="140">
         <f t="shared" si="39"/>
-        <v>44232</v>
+        <v>44313</v>
       </c>
       <c r="AO45" s="140"/>
       <c r="AP45" s="45"/>
@@ -39223,15 +39233,15 @@
       </c>
       <c r="AE46" s="140">
         <f t="shared" si="40"/>
-        <v>44057</v>
+        <v>44066</v>
       </c>
       <c r="AF46" s="140">
         <f t="shared" si="40"/>
-        <v>44078</v>
+        <v>44096</v>
       </c>
       <c r="AG46" s="140">
         <f t="shared" si="40"/>
-        <v>44099</v>
+        <v>44126</v>
       </c>
       <c r="AH46" s="140"/>
       <c r="AI46" s="140"/>
@@ -39241,7 +39251,7 @@
       <c r="AM46" s="140"/>
       <c r="AN46" s="140">
         <f t="shared" si="40"/>
-        <v>44225</v>
+        <v>44306</v>
       </c>
       <c r="AO46" s="140"/>
       <c r="AP46" s="45"/>
@@ -39333,15 +39343,15 @@
       </c>
       <c r="AE47" s="140">
         <f t="shared" si="41"/>
-        <v>44036</v>
+        <v>44045</v>
       </c>
       <c r="AF47" s="140">
         <f t="shared" si="41"/>
-        <v>44057</v>
+        <v>44075</v>
       </c>
       <c r="AG47" s="140">
         <f t="shared" si="41"/>
-        <v>44078</v>
+        <v>44105</v>
       </c>
       <c r="AH47" s="140"/>
       <c r="AI47" s="140"/>
@@ -39351,7 +39361,7 @@
       <c r="AM47" s="140"/>
       <c r="AN47" s="140">
         <f t="shared" si="41"/>
-        <v>44204</v>
+        <v>44285</v>
       </c>
       <c r="AO47" s="140"/>
       <c r="AP47" s="45"/>
@@ -39443,15 +39453,15 @@
       </c>
       <c r="AE48" s="140">
         <f t="shared" si="42"/>
-        <v>44029</v>
+        <v>44038</v>
       </c>
       <c r="AF48" s="140">
         <f t="shared" si="42"/>
-        <v>44050</v>
+        <v>44068</v>
       </c>
       <c r="AG48" s="140">
         <f t="shared" si="42"/>
-        <v>44071</v>
+        <v>44098</v>
       </c>
       <c r="AH48" s="140"/>
       <c r="AI48" s="140"/>
@@ -39461,7 +39471,7 @@
       <c r="AM48" s="140"/>
       <c r="AN48" s="140">
         <f t="shared" si="42"/>
-        <v>44197</v>
+        <v>44278</v>
       </c>
       <c r="AO48" s="140"/>
       <c r="AP48" s="45"/>
@@ -39570,47 +39580,47 @@
       </c>
       <c r="AE51" s="252">
         <f t="shared" si="43"/>
-        <v>30.142857142857142</v>
+        <v>31.428571428571427</v>
       </c>
       <c r="AF51" s="253">
         <f t="shared" si="43"/>
-        <v>33.142857142857146</v>
+        <v>35.714285714285715</v>
       </c>
       <c r="AG51" s="254">
         <f t="shared" si="43"/>
-        <v>36.142857142857146</v>
+        <v>40</v>
       </c>
       <c r="AH51" s="278">
         <f t="shared" ref="AH51:AM51" si="44">(AH28-$B$25)/7</f>
-        <v>39.142857142857146</v>
+        <v>44.285714285714285</v>
       </c>
       <c r="AI51" s="253">
         <f t="shared" si="44"/>
-        <v>42.142857142857146</v>
+        <v>48.571428571428569</v>
       </c>
       <c r="AJ51" s="138">
         <f t="shared" si="44"/>
-        <v>45.142857142857146</v>
+        <v>52.857142857142854</v>
       </c>
       <c r="AK51" s="135">
         <f t="shared" si="44"/>
-        <v>48.142857142857146</v>
+        <v>57.142857142857146</v>
       </c>
       <c r="AL51" s="135">
         <f t="shared" si="44"/>
-        <v>51.142857142857146</v>
+        <v>61.428571428571431</v>
       </c>
       <c r="AM51" s="138">
         <f t="shared" si="44"/>
-        <v>51.142857142857146</v>
+        <v>61.428571428571431</v>
       </c>
       <c r="AN51" s="136">
         <f>(AN28-$B$25)/7</f>
-        <v>54.142857142857146</v>
+        <v>65.714285714285708</v>
       </c>
       <c r="AO51" s="136">
         <f t="shared" si="43"/>
-        <v>62.142857142857146</v>
+        <v>73.714285714285708</v>
       </c>
     </row>
     <row r="52" spans="1:41" s="66" customFormat="1" x14ac:dyDescent="0.25">
@@ -39699,47 +39709,47 @@
       </c>
       <c r="AE52" s="220">
         <f t="shared" si="46"/>
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="AF52" s="220">
         <f t="shared" si="46"/>
-        <v>232</v>
+        <v>250</v>
       </c>
       <c r="AG52" s="220">
         <f t="shared" si="46"/>
-        <v>253</v>
+        <v>280</v>
       </c>
       <c r="AH52" s="220">
         <f t="shared" ref="AH52:AM52" si="47">AH28-$B$25</f>
-        <v>274</v>
+        <v>310</v>
       </c>
       <c r="AI52" s="221">
         <f t="shared" si="47"/>
-        <v>295</v>
+        <v>340</v>
       </c>
       <c r="AJ52" s="221">
         <f t="shared" si="47"/>
-        <v>316</v>
+        <v>370</v>
       </c>
       <c r="AK52" s="221">
         <f t="shared" si="47"/>
-        <v>337</v>
+        <v>400</v>
       </c>
       <c r="AL52" s="177">
         <f t="shared" si="47"/>
-        <v>358</v>
+        <v>430</v>
       </c>
       <c r="AM52" s="251">
         <f t="shared" si="47"/>
-        <v>358</v>
+        <v>430</v>
       </c>
       <c r="AN52" s="251">
         <f t="shared" si="46"/>
-        <v>379</v>
+        <v>460</v>
       </c>
       <c r="AO52" s="177">
         <f t="shared" si="46"/>
-        <v>435</v>
+        <v>516</v>
       </c>
     </row>
     <row r="53" spans="1:41" x14ac:dyDescent="0.25">
@@ -39810,7 +39820,7 @@
         <v>2086864</v>
       </c>
       <c r="AE53" s="259">
-        <f t="shared" ref="AD53:AI53" si="48">AE29</f>
+        <f t="shared" ref="AE53:AI53" si="48">AE29</f>
         <v>4096000</v>
       </c>
       <c r="AF53" s="259">
@@ -39940,47 +39950,47 @@
       </c>
       <c r="AE54" s="172">
         <f t="shared" si="52"/>
-        <v>10.317198946666544</v>
+        <v>10.844782983711992</v>
       </c>
       <c r="AF54" s="172">
         <f t="shared" si="52"/>
-        <v>10.908752407098556</v>
+        <v>11.905491205716698</v>
       </c>
       <c r="AG54" s="172">
         <f t="shared" si="52"/>
-        <v>11.43822949834742</v>
+        <v>12.854890949977603</v>
       </c>
       <c r="AH54" s="172">
         <f t="shared" ref="AH54" si="53">(AH28-$N$28)/(LOG(AH53/$N$53)/LOG(2))</f>
-        <v>11.91491433699685</v>
+        <v>13.709629467255789</v>
       </c>
       <c r="AI54" s="172">
         <f t="shared" ref="AI54" si="54">(AI28-$N$28)/(LOG(AI53/$N$53)/LOG(2))</f>
-        <v>12.346327582020523</v>
+        <v>14.483191971216382</v>
       </c>
       <c r="AJ54" s="172">
         <f t="shared" ref="AJ54" si="55">(AJ28-$N$28)/(LOG(AJ53/$N$53)/LOG(2))</f>
-        <v>12.738626150569033</v>
+        <v>15.186618364557388</v>
       </c>
       <c r="AK54" s="172">
         <f t="shared" ref="AK54:AL54" si="56">(AK28-$N$28)/(LOG(AK53/$N$53)/LOG(2))</f>
-        <v>13.09689892639404</v>
+        <v>15.829033470641804</v>
       </c>
       <c r="AL54" s="175">
         <f t="shared" si="56"/>
-        <v>13.425388722132309</v>
+        <v>16.418045031709791</v>
       </c>
       <c r="AM54" s="175">
         <f t="shared" ref="AM54" si="57">(AM28-$N$28)/(LOG(AM53/$N$53)/LOG(2))</f>
-        <v>13.425388722132309</v>
+        <v>16.418045031709791</v>
       </c>
       <c r="AN54" s="175">
         <f t="shared" si="52"/>
-        <v>13.507261236050558</v>
+        <v>16.687750073608974</v>
       </c>
       <c r="AO54" s="176">
         <f t="shared" si="52"/>
-        <v>15.706117716337859</v>
+        <v>18.886606553896275</v>
       </c>
     </row>
     <row r="55" spans="1:41" x14ac:dyDescent="0.25">
@@ -40146,7 +40156,9 @@
         <f t="shared" si="62"/>
         <v>1424669</v>
       </c>
-      <c r="AE56" s="280"/>
+      <c r="AE56" s="280">
+        <v>2713933</v>
+      </c>
       <c r="AF56" s="280"/>
       <c r="AG56" s="280"/>
       <c r="AH56" s="280"/>
@@ -40225,7 +40237,9 @@
       <c r="AD57" s="277">
         <v>45578</v>
       </c>
-      <c r="AE57" s="281"/>
+      <c r="AE57" s="281">
+        <v>63657</v>
+      </c>
       <c r="AF57" s="281"/>
       <c r="AG57" s="281"/>
       <c r="AH57" s="281"/>
@@ -44993,7 +45007,7 @@
   <dimension ref="B3:J40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45039,7 +45053,7 @@
         <v>118</v>
       </c>
       <c r="C6" s="152">
-        <v>2594112</v>
+        <v>3542733</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
@@ -45048,7 +45062,7 @@
       </c>
       <c r="C7" s="150">
         <f ca="1">NOW()</f>
-        <v>44059.868929861113</v>
+        <v>44073.627557754633</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
@@ -45057,7 +45071,7 @@
       </c>
       <c r="C8" s="151">
         <f ca="1">C7-C5</f>
-        <v>164.86892986111343</v>
+        <v>178.62755775463302</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -45066,7 +45080,7 @@
       </c>
       <c r="C9" s="153">
         <f ca="1">C8/(LOG(C6/C4)/LOG(2))</f>
-        <v>10.089264860751246</v>
+        <v>10.638515448014783</v>
       </c>
       <c r="D9" t="s">
         <v>97</v>
@@ -45099,7 +45113,7 @@
       </c>
       <c r="C12" s="158">
         <f>C6/Projections!B17</f>
-        <v>5707046.3999999994</v>
+        <v>7794012.5999999996</v>
       </c>
     </row>
     <row r="13" spans="2:10" s="66" customFormat="1" x14ac:dyDescent="0.25">
@@ -45108,7 +45122,7 @@
       </c>
       <c r="C13" s="159">
         <f ca="1">(C4/Projections!B17)*(2^(((C7-21)-C5)/C9))</f>
-        <v>1348470.5941363617</v>
+        <v>1983992.5872900242</v>
       </c>
     </row>
     <row r="14" spans="2:10" s="66" customFormat="1" x14ac:dyDescent="0.25">
@@ -45117,7 +45131,7 @@
       </c>
       <c r="C14" s="141">
         <f ca="1">C12-C13</f>
-        <v>4358575.8058636375</v>
+        <v>5810020.0127099752</v>
       </c>
       <c r="E14" s="155"/>
       <c r="F14" s="156" t="s">
@@ -45131,7 +45145,7 @@
       </c>
       <c r="C15" s="63">
         <f>C6*Projections!B21</f>
-        <v>2101230.7200000002</v>
+        <v>2869613.73</v>
       </c>
       <c r="I15" s="149"/>
     </row>
@@ -45141,7 +45155,7 @@
       </c>
       <c r="C16" s="77">
         <f ca="1">(C4*Projections!B21)*(2^(((C7-21)-C5)/C9))</f>
-        <v>496482.35511384223</v>
+        <v>730469.99804769072</v>
       </c>
       <c r="I16" s="149"/>
     </row>
@@ -45151,7 +45165,7 @@
       </c>
       <c r="C17" s="77">
         <f ca="1">C15-C16</f>
-        <v>1604748.3648861579</v>
+        <v>2139143.7319523091</v>
       </c>
       <c r="F17" t="s">
         <v>142</v>
@@ -45164,7 +45178,7 @@
       </c>
       <c r="C18" s="63">
         <f>C6*Projections!B22</f>
-        <v>363175.68000000005</v>
+        <v>495982.62000000005</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -45173,7 +45187,7 @@
       </c>
       <c r="C19" s="77">
         <f ca="1">(C4*Projections!B22)*(2^(((C7-49)-C5)/C9))</f>
-        <v>12534.882603669403</v>
+        <v>20368.106425737344</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -45182,7 +45196,7 @@
       </c>
       <c r="C20" s="77">
         <f ca="1">C18-C19</f>
-        <v>350640.79739633063</v>
+        <v>475614.51357426273</v>
       </c>
       <c r="F20" t="s">
         <v>147</v>
@@ -45194,7 +45208,7 @@
       </c>
       <c r="C21" s="63">
         <f>C6*Projections!B23</f>
-        <v>129705.60000000001</v>
+        <v>177136.65000000002</v>
       </c>
       <c r="I21" s="149"/>
     </row>
@@ -45204,7 +45218,7 @@
       </c>
       <c r="C22" s="77">
         <f ca="1">(C4*Projections!B23)*(2^(((C7-49)-C5)/C9))</f>
-        <v>4476.7437870247868</v>
+        <v>7274.3237234776234</v>
       </c>
       <c r="I22" s="149"/>
     </row>
@@ -45214,7 +45228,7 @@
       </c>
       <c r="C23" s="77">
         <f ca="1">C21-C22</f>
-        <v>125228.85621297522</v>
+        <v>169862.32627652239</v>
       </c>
       <c r="I23" s="149"/>
     </row>
@@ -45224,7 +45238,7 @@
       </c>
       <c r="C24" s="63">
         <f>C6*Projections!B24</f>
-        <v>57070.464</v>
+        <v>77940.125999999989</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
@@ -45233,7 +45247,7 @@
       </c>
       <c r="C25" s="60">
         <f ca="1">(C4*Projections!B24)*(2^(((C7-42)-C5)/C9))</f>
-        <v>3186.189170024054</v>
+        <v>5050.3210456983015</v>
       </c>
       <c r="F25" t="s">
         <v>153</v>
@@ -45245,7 +45259,7 @@
       </c>
       <c r="C26" s="162">
         <f ca="1">C9*(LOG(C10/C21)/LOG(2))</f>
-        <v>24.326334908868407</v>
+        <v>20.867328614801551</v>
       </c>
       <c r="D26" t="s">
         <v>97</v>
@@ -45260,7 +45274,7 @@
       </c>
       <c r="C27" s="161">
         <f ca="1">C7+C26</f>
-        <v>44084.19526476998</v>
+        <v>44094.494886369437</v>
       </c>
       <c r="F27" t="s">
         <v>155</v>
@@ -45272,7 +45286,7 @@
       </c>
       <c r="C28" s="160">
         <f ca="1">C9*(LOG(C11/C21)/LOG(2))</f>
-        <v>-14.481565755505013</v>
+        <v>-20.053239575358774</v>
       </c>
       <c r="D28" t="s">
         <v>97</v>
@@ -45284,7 +45298,7 @@
       </c>
       <c r="C29" s="161">
         <f ca="1">C7+C28</f>
-        <v>44045.387364105605</v>
+        <v>44053.574318179271</v>
       </c>
       <c r="F29" t="s">
         <v>155</v>
@@ -45296,7 +45310,7 @@
       </c>
       <c r="C30" s="160">
         <f ca="1">C9*(LOG((C3*0.6)/C12)/LOG(2))</f>
-        <v>72.576070241704713</v>
+        <v>71.743736538022915</v>
       </c>
       <c r="D30" t="s">
         <v>97</v>
@@ -45308,7 +45322,7 @@
       </c>
       <c r="C31" s="161">
         <f ca="1">C7+C30</f>
-        <v>44132.445000102816</v>
+        <v>44145.371294292658</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
@@ -45317,7 +45331,7 @@
       </c>
       <c r="C34" s="150">
         <f ca="1">C7+30</f>
-        <v>44089.868929861113</v>
+        <v>44103.627557754633</v>
       </c>
       <c r="F34" t="s">
         <v>168</v>
@@ -45329,7 +45343,7 @@
       </c>
       <c r="C35" s="77">
         <f ca="1">C6*(2^((C34-C7)/C9))</f>
-        <v>20374577.559489168</v>
+        <v>25016448.185279295</v>
       </c>
       <c r="F35" t="s">
         <v>140</v>
@@ -45341,7 +45355,7 @@
       </c>
       <c r="C36" s="77">
         <f ca="1">C35/Projections!B17</f>
-        <v>44824070.630876169</v>
+        <v>55036186.007614441</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
@@ -45350,7 +45364,7 @@
       </c>
       <c r="C37" s="77">
         <f ca="1">C35*Projections!B21</f>
-        <v>16503407.823186228</v>
+        <v>20263323.030076232</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
@@ -45359,7 +45373,7 @@
       </c>
       <c r="C38" s="77">
         <f ca="1">C35*Projections!B22</f>
-        <v>2852440.858328484</v>
+        <v>3502302.7459391016</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
@@ -45368,7 +45382,7 @@
       </c>
       <c r="C39" s="77">
         <f ca="1">C35*Projections!B23</f>
-        <v>1018728.8779744585</v>
+        <v>1250822.4092639647</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
@@ -45377,7 +45391,7 @@
       </c>
       <c r="C40" s="60">
         <f ca="1">C35*Projections!B24</f>
-        <v>448240.70630876167</v>
+        <v>550361.86007614445</v>
       </c>
     </row>
   </sheetData>

</xml_diff>